<commit_message>
Removed unwanted excel & java file / and added duplicate excel
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="267">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -633,6 +633,210 @@
   </si>
   <si>
     <t>Name&lt;column&gt;Title&lt;column&gt;Email&lt;break&gt;Staff Name&lt;column&gt;Title&lt;column&gt;Mobile Phone</t>
+  </si>
+  <si>
+    <t>FC2</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Test Demo 1</t>
+  </si>
+  <si>
+    <t>FC3</t>
+  </si>
+  <si>
+    <t>Test Demo 2</t>
+  </si>
+  <si>
+    <t>FC4</t>
+  </si>
+  <si>
+    <t>Test Demo 3</t>
+  </si>
+  <si>
+    <t>FC5</t>
+  </si>
+  <si>
+    <t>Test Demo 4</t>
+  </si>
+  <si>
+    <t>FC6</t>
+  </si>
+  <si>
+    <t>Test Demo 5</t>
+  </si>
+  <si>
+    <t>FC7</t>
+  </si>
+  <si>
+    <t>Test Demo 6</t>
+  </si>
+  <si>
+    <t>FC8</t>
+  </si>
+  <si>
+    <t>Test Demo 7</t>
+  </si>
+  <si>
+    <t>FC9</t>
+  </si>
+  <si>
+    <t>Test Demo 8</t>
+  </si>
+  <si>
+    <t>FC10</t>
+  </si>
+  <si>
+    <t>Test Demo 9</t>
+  </si>
+  <si>
+    <t>FC11</t>
+  </si>
+  <si>
+    <t>Test Demo 10</t>
+  </si>
+  <si>
+    <t>Deal Demo 1</t>
+  </si>
+  <si>
+    <t>Deal Demo 2</t>
+  </si>
+  <si>
+    <t>Deal Demo 3</t>
+  </si>
+  <si>
+    <t>Deal Demo 4</t>
+  </si>
+  <si>
+    <t>Deal Demo 5</t>
+  </si>
+  <si>
+    <t>Deal Demo 6</t>
+  </si>
+  <si>
+    <t>Deal Demo 7</t>
+  </si>
+  <si>
+    <t>Deal Demo 8</t>
+  </si>
+  <si>
+    <t>Deal Demo 9</t>
+  </si>
+  <si>
+    <t>Deal Demo 10</t>
+  </si>
+  <si>
+    <t>FC12</t>
+  </si>
+  <si>
+    <t>FC13</t>
+  </si>
+  <si>
+    <t>FC14</t>
+  </si>
+  <si>
+    <t>FC15</t>
+  </si>
+  <si>
+    <t>FC16</t>
+  </si>
+  <si>
+    <t>FC17</t>
+  </si>
+  <si>
+    <t>FC18</t>
+  </si>
+  <si>
+    <t>FC19</t>
+  </si>
+  <si>
+    <t>FC20</t>
+  </si>
+  <si>
+    <t>FC21</t>
+  </si>
+  <si>
+    <t>Event Demo 1</t>
+  </si>
+  <si>
+    <t>Event Demo 2</t>
+  </si>
+  <si>
+    <t>Event Demo 3</t>
+  </si>
+  <si>
+    <t>Event Demo 4</t>
+  </si>
+  <si>
+    <t>Event Demo 5</t>
+  </si>
+  <si>
+    <t>Event Demo 6</t>
+  </si>
+  <si>
+    <t>Event Demo 7</t>
+  </si>
+  <si>
+    <t>Event Demo 8</t>
+  </si>
+  <si>
+    <t>Event Demo 9</t>
+  </si>
+  <si>
+    <t>Event Demo 10</t>
+  </si>
+  <si>
+    <t>Marketing Event</t>
+  </si>
+  <si>
+    <t>FC22</t>
+  </si>
+  <si>
+    <t>FC23</t>
+  </si>
+  <si>
+    <t>FC24</t>
+  </si>
+  <si>
+    <t>FC25</t>
+  </si>
+  <si>
+    <t>FC26</t>
+  </si>
+  <si>
+    <t>FC27</t>
+  </si>
+  <si>
+    <t>FC28</t>
+  </si>
+  <si>
+    <t>FC29</t>
+  </si>
+  <si>
+    <t>FC30</t>
+  </si>
+  <si>
+    <t>FC31</t>
+  </si>
+  <si>
+    <t>TestAlexa Sep Deal 2020</t>
+  </si>
+  <si>
+    <t>TestOct Alexa Deal 2021</t>
+  </si>
+  <si>
+    <t>Deal2</t>
+  </si>
+  <si>
+    <t>Deal3</t>
+  </si>
+  <si>
+    <t>CDINS3</t>
+  </si>
+  <si>
+    <t>Apex Corp</t>
   </si>
 </sst>
 </file>
@@ -642,7 +846,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -685,6 +889,12 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1413,7 +1623,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1514,16 +1726,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
@@ -1570,7 +1782,518 @@
         <v>43</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>211</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>200</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" t="s">
+        <v>213</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>219</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>220</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>221</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>222</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>226</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>251</v>
+      </c>
+      <c r="B23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" t="s">
+        <v>240</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>252</v>
+      </c>
+      <c r="B24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>241</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>242</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>254</v>
+      </c>
+      <c r="B26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>243</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>255</v>
+      </c>
+      <c r="B27" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>244</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" t="s">
+        <v>250</v>
+      </c>
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" t="s">
+        <v>245</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>257</v>
+      </c>
+      <c r="B29" t="s">
+        <v>250</v>
+      </c>
+      <c r="C29" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" t="s">
+        <v>246</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>258</v>
+      </c>
+      <c r="B30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" t="s">
+        <v>247</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>259</v>
+      </c>
+      <c r="B31" t="s">
+        <v>250</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>248</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>260</v>
+      </c>
+      <c r="B32" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1579,8 +2302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,7 +3441,18 @@
         <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1003" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3999,13 +4733,13 @@
   <dimension ref="A1:AML7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
@@ -5074,6 +5808,34 @@
         <v>29</v>
       </c>
     </row>
+    <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>153</v>
@@ -5087,6 +5849,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5214,8 +5977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Excel related to Module 3
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="307">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -837,6 +837,126 @@
   </si>
   <si>
     <t>Apex Corp</t>
+  </si>
+  <si>
+    <t>TestAlexa Event 1</t>
+  </si>
+  <si>
+    <t>ME1</t>
+  </si>
+  <si>
+    <t>HSRPIP1</t>
+  </si>
+  <si>
+    <t>TCS-Pipeline</t>
+  </si>
+  <si>
+    <t>Patel Sons</t>
+  </si>
+  <si>
+    <t>Samantha Rao</t>
+  </si>
+  <si>
+    <t>Ajio Trand</t>
+  </si>
+  <si>
+    <t>HSRPIP2</t>
+  </si>
+  <si>
+    <t>Reliance Trade</t>
+  </si>
+  <si>
+    <t>HSRPIP3</t>
+  </si>
+  <si>
+    <t>IriesIndia- pipeline</t>
+  </si>
+  <si>
+    <t>LOI</t>
+  </si>
+  <si>
+    <t>Iries India</t>
+  </si>
+  <si>
+    <t>HSRPIP4</t>
+  </si>
+  <si>
+    <t>NIIT-Pipeline</t>
+  </si>
+  <si>
+    <t>NDA Signed</t>
+  </si>
+  <si>
+    <t>Jinu Alex</t>
+  </si>
+  <si>
+    <t>HSRPIP5</t>
+  </si>
+  <si>
+    <t>Patel Property Deal</t>
+  </si>
+  <si>
+    <t>Anuradha Jaiswal</t>
+  </si>
+  <si>
+    <t>Sharda Firms</t>
+  </si>
+  <si>
+    <t>HSRCON1</t>
+  </si>
+  <si>
+    <t>Samantha</t>
+  </si>
+  <si>
+    <t>Rao</t>
+  </si>
+  <si>
+    <t>navatariptesting+33853@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRCON2</t>
+  </si>
+  <si>
+    <t>Jinu</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>navatariptesting+13818@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRCON3</t>
+  </si>
+  <si>
+    <t>Anuradha</t>
+  </si>
+  <si>
+    <t>Jaiswal</t>
+  </si>
+  <si>
+    <t>Kanya Groups</t>
+  </si>
+  <si>
+    <t>navatariptesting+78464@gmail.com</t>
+  </si>
+  <si>
+    <t>HSRINS1</t>
+  </si>
+  <si>
+    <t>Intermediary</t>
+  </si>
+  <si>
+    <t>HSRINS2</t>
+  </si>
+  <si>
+    <t>HSRINS3</t>
+  </si>
+  <si>
+    <t>HSRINS4</t>
+  </si>
+  <si>
+    <t>HSRINS5</t>
   </si>
 </sst>
 </file>
@@ -846,7 +966,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -883,12 +1003,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="8"/>
@@ -942,7 +1056,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -993,7 +1107,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1376,7 +1489,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E18" activeCellId="1" sqref="E3 E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1498,7 @@
     <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -1424,7 +1537,21 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="28"/>
+      <c r="A3" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2293,17 +2420,17 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO17"/>
+  <dimension ref="A1:ALO23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,6 +3593,61 @@
         <v>35</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3473,10 +3655,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR8"/>
+  <dimension ref="A1:ALR12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4616,6 +4798,57 @@
         <v>124</v>
       </c>
     </row>
+    <row r="10" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>289</v>
+      </c>
+      <c r="C10" t="s">
+        <v>290</v>
+      </c>
+      <c r="D10" t="s">
+        <v>273</v>
+      </c>
+      <c r="E10" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C11" t="s">
+        <v>294</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D12" t="s">
+        <v>299</v>
+      </c>
+      <c r="E12" t="s">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4623,10 +4856,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4635,13 +4868,14 @@
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -4654,20 +4888,23 @@
       <c r="D1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -4681,7 +4918,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -4695,7 +4932,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>150</v>
       </c>
@@ -4709,7 +4946,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>152</v>
       </c>
@@ -4730,10 +4967,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML7"/>
+  <dimension ref="A1:AML14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5848,8 +6085,108 @@
         <v>32</v>
       </c>
     </row>
+    <row r="10" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>269</v>
+      </c>
+      <c r="B10" t="s">
+        <v>270</v>
+      </c>
+      <c r="C10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" t="s">
+        <v>271</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>276</v>
+      </c>
+      <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
+        <v>271</v>
+      </c>
+      <c r="D12" t="s">
+        <v>278</v>
+      </c>
+      <c r="E12" t="s">
+        <v>272</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B13" t="s">
+        <v>281</v>
+      </c>
+      <c r="C13" t="s">
+        <v>271</v>
+      </c>
+      <c r="D13" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>284</v>
+      </c>
+      <c r="B14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" t="s">
+        <v>271</v>
+      </c>
+      <c r="D14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E14" t="s">
+        <v>286</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Excel updated M3 TC017-020
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -9,22 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId2"/>
-    <sheet name="Entities" sheetId="3" r:id="rId3"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId4"/>
-    <sheet name="Fund" sheetId="7" r:id="rId5"/>
-    <sheet name="Deal" sheetId="4" r:id="rId6"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId7"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId8"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId9"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId10"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId11"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId12"/>
-    <sheet name="Task" sheetId="12" r:id="rId13"/>
+    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
+    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
+    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
+    <sheet name="Entities" sheetId="3" r:id="rId4"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
+    <sheet name="Fund" sheetId="7" r:id="rId6"/>
+    <sheet name="Deal" sheetId="4" r:id="rId7"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId8"/>
+    <sheet name="CustomSDG" sheetId="13" r:id="rId9"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId10"/>
+    <sheet name="MarketingEvent" sheetId="15" r:id="rId11"/>
+    <sheet name="Partnerships" sheetId="8" r:id="rId12"/>
+    <sheet name="Commitments" sheetId="9" r:id="rId13"/>
+    <sheet name="Task" sheetId="12" r:id="rId14"/>
+    <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="347">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -957,6 +959,126 @@
   </si>
   <si>
     <t>HSRINS5</t>
+  </si>
+  <si>
+    <t>Image_Field_Name</t>
+  </si>
+  <si>
+    <t>PageLayOut_API_Name</t>
+  </si>
+  <si>
+    <t>Field_Name</t>
+  </si>
+  <si>
+    <t>UD1</t>
+  </si>
+  <si>
+    <t>Profile_Image__c</t>
+  </si>
+  <si>
+    <t>Profile_Image</t>
+  </si>
+  <si>
+    <t>UD2</t>
+  </si>
+  <si>
+    <t>Pipeline Layout</t>
+  </si>
+  <si>
+    <t>Profile Image</t>
+  </si>
+  <si>
+    <t>UD3</t>
+  </si>
+  <si>
+    <t>Marketing_Event</t>
+  </si>
+  <si>
+    <t>Firm Events</t>
+  </si>
+  <si>
+    <t>TestCases_Name</t>
+  </si>
+  <si>
+    <t>Navigation_Label_Name</t>
+  </si>
+  <si>
+    <t>Redirection_Label_Name</t>
+  </si>
+  <si>
+    <t>Update_Navigation_Label_Name</t>
+  </si>
+  <si>
+    <t>Updated_Order</t>
+  </si>
+  <si>
+    <t>Module3Tc009_1_UpdateReportsAndDashboardURLWithAnActualReporAndDashboardLink_Action</t>
+  </si>
+  <si>
+    <t>Reports&lt;break&gt;Dashboards</t>
+  </si>
+  <si>
+    <t>Account Referrals&lt;break&gt;Dead Deals</t>
+  </si>
+  <si>
+    <t>Module3Tc011_RenameNavigationLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Fund&lt;break&gt;Contact</t>
+  </si>
+  <si>
+    <t>New Fund&lt;break&gt;New Contact</t>
+  </si>
+  <si>
+    <t>Module3Tc012_ChangeTheOrderOfTheLabelAndVerifyImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>New Contact&lt;break&gt;Reports&lt;break&gt;Fund Manager&lt;break&gt;Institution&lt;break&gt;Partnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40&lt;break&gt;-10&lt;break&gt;5&lt;break&gt;-10&lt;break&gt; </t>
+  </si>
+  <si>
+    <t>FieldSetLabel</t>
+  </si>
+  <si>
+    <t>Fund Preferences&lt;break&gt;Existing LP&lt;break&gt;Fund Commitments (mn)&lt;break&gt;Total Co-investment Commitments (mn)&lt;break&gt;Industry&lt;break&gt;Region</t>
+  </si>
+  <si>
+    <t>Log In Date&lt;break&gt;Revenue&lt;break&gt;EBITDA&lt;break&gt;Industry&lt;break&gt;Region&lt;break&gt;Stage</t>
+  </si>
+  <si>
+    <t>Display_field_set</t>
+  </si>
+  <si>
+    <t>Date&lt;break&gt;Type&lt;break&gt;Status&lt;break&gt;Location&lt;break&gt;Main Contact&lt;break&gt;Region</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Module3Tc015_1_AddNewNavigationItemsAndVerifyItOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Dashboards</t>
+  </si>
+  <si>
+    <t>Module3Tc018_CreateSubMenuAndVerify</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Module3Tc019_CreateSubMenuForIIndlevelAndVerifyItOnTheNavigationMenu</t>
+  </si>
+  <si>
+    <t>Test Label 2,10,Reports,,,,,</t>
   </si>
 </sst>
 </file>
@@ -966,7 +1088,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,6 +1131,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1056,7 +1184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1107,6 +1235,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1388,94 +1517,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>50</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>322</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
+      <c r="A3" s="14" t="s">
+        <v>327</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>34</v>
+        <v>328</v>
+      </c>
+      <c r="D3" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>23</v>
+      <c r="A4" s="14" t="s">
+        <v>330</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>331</v>
+      </c>
+      <c r="E4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" t="s">
+        <v>343</v>
+      </c>
+      <c r="F6" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -1486,10 +1619,114 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" activeCellId="1" sqref="E3 E18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1616,7 +1853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1746,12 +1983,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1851,7 +2088,247 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" t="s">
+        <v>334</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>314</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="H3" t="s">
+        <v>335</v>
+      </c>
+      <c r="I3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" t="s">
+        <v>318</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>315</v>
+      </c>
+      <c r="H4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
@@ -2425,7 +2902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO23"/>
   <sheetViews>
@@ -3653,7 +4130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR12"/>
   <sheetViews>
@@ -4854,11 +5331,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4965,7 +5442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML14"/>
   <sheetViews>
@@ -6191,7 +6668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -6261,7 +6738,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6308,108 +6785,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>198</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Excel updated for Module 3 tc024-30
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -27,6 +27,7 @@
     <sheet name="Commitments" sheetId="9" r:id="rId13"/>
     <sheet name="Task" sheetId="12" r:id="rId14"/>
     <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
+    <sheet name="Fields" sheetId="19" r:id="rId16"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="409">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -886,9 +887,6 @@
     <t>NIIT-Pipeline</t>
   </si>
   <si>
-    <t>NDA Signed</t>
-  </si>
-  <si>
     <t>Jinu Alex</t>
   </si>
   <si>
@@ -1079,6 +1077,195 @@
   </si>
   <si>
     <t>Test Label 2,10,Reports,,,,,</t>
+  </si>
+  <si>
+    <t>Non-Disclosure Agreement</t>
+  </si>
+  <si>
+    <t>Parent_Field_Name</t>
+  </si>
+  <si>
+    <t>accountId</t>
+  </si>
+  <si>
+    <t>M4SDG1</t>
+  </si>
+  <si>
+    <t>M4SDG2</t>
+  </si>
+  <si>
+    <t>Deal Team</t>
+  </si>
+  <si>
+    <t>Deal_Team__c</t>
+  </si>
+  <si>
+    <t>Pipeline__c</t>
+  </si>
+  <si>
+    <t>APIName</t>
+  </si>
+  <si>
+    <t>Override_Label</t>
+  </si>
+  <si>
+    <t>FieldOrder</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>navpeII__Contact_Referral_Source__c</t>
+  </si>
+  <si>
+    <t>Contact Referral Source</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Attendee_Staff__r.Name</t>
+  </si>
+  <si>
+    <t>Attendee_Staff__r.Title</t>
+  </si>
+  <si>
+    <t>Status__c</t>
+  </si>
+  <si>
+    <t>Notes__c</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>CField1</t>
+  </si>
+  <si>
+    <t>CField2</t>
+  </si>
+  <si>
+    <t>CField3</t>
+  </si>
+  <si>
+    <t>CField4</t>
+  </si>
+  <si>
+    <t>CField5</t>
+  </si>
+  <si>
+    <t>DTField1</t>
+  </si>
+  <si>
+    <t>DTField2</t>
+  </si>
+  <si>
+    <t>AFIeld1</t>
+  </si>
+  <si>
+    <t>AField2</t>
+  </si>
+  <si>
+    <t>AField3</t>
+  </si>
+  <si>
+    <t>AField4</t>
+  </si>
+  <si>
+    <t>DTField3</t>
+  </si>
+  <si>
+    <t>DTField4</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>M4SDG3</t>
+  </si>
+  <si>
+    <t>Attendee</t>
+  </si>
+  <si>
+    <t>Attendee__c</t>
+  </si>
+  <si>
+    <t>Marketing_Event__c</t>
+  </si>
+  <si>
+    <t>Navigation_Label_With_Parent</t>
+  </si>
+  <si>
+    <t>List_View_Object</t>
+  </si>
+  <si>
+    <t>List_View_Name</t>
+  </si>
+  <si>
+    <t>Module3Tc021_FillThirdPartyWebsiteToReportAndDashboardAndVerifyTheNavigation</t>
+  </si>
+  <si>
+    <t>Accounts/Reports&lt;break&gt;Dashboards</t>
+  </si>
+  <si>
+    <t>Module3Tc022_CreateListViewAndVerifyTheNavigationForListView</t>
+  </si>
+  <si>
+    <t>Marketing Prospects</t>
+  </si>
+  <si>
+    <t>navpeII__Marketing_Prospect__c</t>
+  </si>
+  <si>
+    <t>Automation_All</t>
+  </si>
+  <si>
+    <t>Module3Tc023_CreateALightningAppPageAndVerifyTheNavigationForLighteningAppPage</t>
+  </si>
+  <si>
+    <t>Custom Label 2</t>
+  </si>
+  <si>
+    <t>Accounts/Custom Label 2</t>
+  </si>
+  <si>
+    <t>Module3Tc024_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>OtherAccount</t>
+  </si>
+  <si>
+    <t>Institution&lt;break&gt;Company&lt;break&gt;Fund Manager&lt;break&gt;Fund Manager’s Fund&lt;break&gt;Individual Investor&lt;break&gt;Intermediary&lt;break&gt;Limited Partner</t>
+  </si>
+  <si>
+    <t>Module3Tc025_FillTheRecordTypeIDAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Intermediary&lt;break&gt;Individual Investor&lt;break&gt;Limited Partner</t>
+  </si>
+  <si>
+    <t>Module3Tc027_RemoveTheRecordTypeAPIFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc028_FillSomeThirdPartyUrlInUrlFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc029_CreateAlistViewOfAccountsAndListViewInformationOnNavigationPage</t>
+  </si>
+  <si>
+    <t>Module3Tc030_RemoveTheURLAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc031_RemoveQuickCreateObjectFieldAndVerifyTheImpactOnNavigationMenu</t>
   </si>
 </sst>
 </file>
@@ -1517,98 +1704,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="66" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>321</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="13" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="B5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" t="s">
+        <v>342</v>
+      </c>
+      <c r="F6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B7" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" t="s">
         <v>324</v>
       </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="B3" t="s">
-        <v>328</v>
-      </c>
-      <c r="D3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="B4" t="s">
-        <v>331</v>
-      </c>
-      <c r="E4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="B5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="B6" t="s">
-        <v>343</v>
-      </c>
-      <c r="F6" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="B7" t="s">
-        <v>346</v>
+      <c r="G8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="B9" t="s">
+        <v>393</v>
+      </c>
+      <c r="H9" t="s">
+        <v>394</v>
+      </c>
+      <c r="I9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="B10" t="s">
+        <v>397</v>
+      </c>
+      <c r="G10" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>399</v>
+      </c>
+      <c r="B11" t="s">
+        <v>400</v>
+      </c>
+      <c r="J11" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="B12" t="s">
+        <v>400</v>
+      </c>
+      <c r="J12" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="B13" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="B14" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>406</v>
+      </c>
+      <c r="B15" t="s">
+        <v>400</v>
+      </c>
+      <c r="I15" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="B16" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B17" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -1987,9 +2291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2120,27 +2422,27 @@
         <v>180</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>309</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B2" t="s">
         <v>185</v>
@@ -2149,7 +2451,7 @@
         <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E2" t="s">
         <v>200</v>
@@ -2158,10 +2460,10 @@
         <v>35</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I2" t="s">
         <v>35</v>
@@ -2169,7 +2471,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B3" t="s">
         <v>190</v>
@@ -2178,27 +2480,27 @@
         <v>262</v>
       </c>
       <c r="D3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G3" s="28" t="s">
         <v>314</v>
       </c>
-      <c r="G3" s="28" t="s">
-        <v>315</v>
-      </c>
       <c r="H3" t="s">
+        <v>334</v>
+      </c>
+      <c r="I3" t="s">
         <v>335</v>
-      </c>
-      <c r="I3" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" t="s">
         <v>195</v>
@@ -2207,22 +2509,246 @@
         <v>267</v>
       </c>
       <c r="D4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E4" t="s">
+        <v>316</v>
+      </c>
+      <c r="F4" t="s">
         <v>317</v>
       </c>
-      <c r="F4" t="s">
-        <v>318</v>
-      </c>
       <c r="G4" s="28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H4" t="s">
+        <v>336</v>
+      </c>
+      <c r="I4" t="s">
         <v>337</v>
       </c>
-      <c r="I4" t="s">
-        <v>338</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
+        <v>358</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B4" t="s">
+        <v>360</v>
+      </c>
+      <c r="C4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>372</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>373</v>
+      </c>
+      <c r="B6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C6" t="s">
+        <v>362</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>374</v>
+      </c>
+      <c r="B7" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" t="s">
+        <v>358</v>
+      </c>
+      <c r="C8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>381</v>
+      </c>
+      <c r="B10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" t="s">
+        <v>364</v>
+      </c>
+      <c r="C11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12" t="s">
+        <v>365</v>
+      </c>
+      <c r="C12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" t="s">
+        <v>366</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>379</v>
+      </c>
+      <c r="B14" t="s">
+        <v>367</v>
+      </c>
+      <c r="C14" t="s">
+        <v>368</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2906,7 +3432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -4072,29 +4598,29 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>273</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B20" s="22" t="s">
         <v>279</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>271</v>
@@ -4105,10 +4631,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -4116,13 +4642,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -4135,7 +4661,7 @@
   <dimension ref="A1:ALR12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5277,53 +5803,53 @@
     </row>
     <row r="10" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>287</v>
+      </c>
+      <c r="B10" t="s">
         <v>288</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>289</v>
-      </c>
-      <c r="C10" t="s">
-        <v>290</v>
       </c>
       <c r="D10" t="s">
         <v>273</v>
       </c>
       <c r="E10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="11" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>291</v>
+      </c>
+      <c r="B11" t="s">
         <v>292</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>293</v>
-      </c>
-      <c r="C11" t="s">
-        <v>294</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>279</v>
       </c>
       <c r="E11" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="12" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" t="s">
         <v>296</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>297</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>298</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>299</v>
-      </c>
-      <c r="E12" t="s">
-        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5447,7 +5973,7 @@
   <dimension ref="A1:AML14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6633,10 +7159,10 @@
         <v>271</v>
       </c>
       <c r="D13" t="s">
+        <v>346</v>
+      </c>
+      <c r="E13" t="s">
         <v>282</v>
-      </c>
-      <c r="E13" t="s">
-        <v>283</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>279</v>
@@ -6644,10 +7170,10 @@
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" t="s">
         <v>284</v>
-      </c>
-      <c r="B14" t="s">
-        <v>285</v>
       </c>
       <c r="C14" t="s">
         <v>271</v>
@@ -6656,10 +7182,10 @@
         <v>278</v>
       </c>
       <c r="E14" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>286</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -6740,10 +7266,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6754,7 +7280,7 @@
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -6767,8 +7293,11 @@
       <c r="D1" s="25" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="25" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>158</v>
       </c>
@@ -6780,6 +7309,57 @@
       </c>
       <c r="D2" s="5" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel for Module 3 TC045-059
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -28,6 +28,8 @@
     <sheet name="Task" sheetId="12" r:id="rId14"/>
     <sheet name="UploadImageData" sheetId="17" r:id="rId15"/>
     <sheet name="Fields" sheetId="19" r:id="rId16"/>
+    <sheet name="Attendees" sheetId="20" r:id="rId17"/>
+    <sheet name="Deal Team" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="510">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1127,9 +1129,6 @@
     <t>navpeII__Contact_Referral_Source__c</t>
   </si>
   <si>
-    <t>Contact Referral Source</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -1266,6 +1265,312 @@
   </si>
   <si>
     <t>Module3Tc031_RemoveQuickCreateObjectFieldAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M4CON1</t>
+  </si>
+  <si>
+    <t>Test Entity1</t>
+  </si>
+  <si>
+    <t>navatariptesting+77479@gmail.com</t>
+  </si>
+  <si>
+    <t>Investor</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>M4CON2</t>
+  </si>
+  <si>
+    <t>navatariptesting+14649@gmail.com</t>
+  </si>
+  <si>
+    <t>Advisor</t>
+  </si>
+  <si>
+    <t>M4CON3</t>
+  </si>
+  <si>
+    <t>navatariptesting+57115@gmail.com</t>
+  </si>
+  <si>
+    <t>M4CON4</t>
+  </si>
+  <si>
+    <t>navatariptesting+18612@gmail.com</t>
+  </si>
+  <si>
+    <t>M4CON5</t>
+  </si>
+  <si>
+    <t>Contact5</t>
+  </si>
+  <si>
+    <t>M4CON6</t>
+  </si>
+  <si>
+    <t>Contact6</t>
+  </si>
+  <si>
+    <t>M4CON7</t>
+  </si>
+  <si>
+    <t>Contact7</t>
+  </si>
+  <si>
+    <t>M4Deal1</t>
+  </si>
+  <si>
+    <t>Deal 1</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.Email</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRoleId</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRole.Nam</t>
+  </si>
+  <si>
+    <t>Attendee_Staff</t>
+  </si>
+  <si>
+    <t>M4Att1</t>
+  </si>
+  <si>
+    <t>PE Admin</t>
+  </si>
+  <si>
+    <t>Invited</t>
+  </si>
+  <si>
+    <t>Event 1</t>
+  </si>
+  <si>
+    <t>Salesforce.com, inc. is an American cloud-based software company headquartered in San Francisco, California. It provides (CRM) customer relationship management service and also sells a complementary suite of enterprise applications focused on customer service, marketing automation, analytics, and application development.</t>
+  </si>
+  <si>
+    <t>M4Att2</t>
+  </si>
+  <si>
+    <t>M4Att3</t>
+  </si>
+  <si>
+    <t>M4Att4</t>
+  </si>
+  <si>
+    <t>M4Att5</t>
+  </si>
+  <si>
+    <t>M4Att6</t>
+  </si>
+  <si>
+    <t>DTID</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>M4DT1</t>
+  </si>
+  <si>
+    <t>Our Advisor</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>M4DT2</t>
+  </si>
+  <si>
+    <t>Company Team</t>
+  </si>
+  <si>
+    <t>M4DT3</t>
+  </si>
+  <si>
+    <t>Company Advisor</t>
+  </si>
+  <si>
+    <t>M4DT4</t>
+  </si>
+  <si>
+    <t>M4DT5</t>
+  </si>
+  <si>
+    <t>M4DT6</t>
+  </si>
+  <si>
+    <t>M4DT7</t>
+  </si>
+  <si>
+    <t>M4DT8</t>
+  </si>
+  <si>
+    <t>M4DT9</t>
+  </si>
+  <si>
+    <t>M4DT10</t>
+  </si>
+  <si>
+    <t>M4DT11</t>
+  </si>
+  <si>
+    <t>M4ME1</t>
+  </si>
+  <si>
+    <t>M4INS1</t>
+  </si>
+  <si>
+    <t>M4INS2</t>
+  </si>
+  <si>
+    <t>Test Entity4</t>
+  </si>
+  <si>
+    <t>Action_Object</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Module3Tc032_RemoveListViewObjectAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc033_RemoveListViewNameAndVerifyTheImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc034_CreateRecordTypeFundAndFundOfFundsForFundObjectAndAddTheFromTheProfiles</t>
+  </si>
+  <si>
+    <t>New Fund</t>
+  </si>
+  <si>
+    <t>navpeII__Fund__c</t>
+  </si>
+  <si>
+    <t>Fund&lt;break&gt;Fund of Funds</t>
+  </si>
+  <si>
+    <t>Module3Tc035_VerifyQuickCreateObjectWhenRecordHasMultipleRecordTypes</t>
+  </si>
+  <si>
+    <t>Module3Tc036_1_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>Module3Tc036_2_UpdateTheRecordTypeAndDescriptionImpactOnNavigationMenu</t>
+  </si>
+  <si>
+    <t>M4Field1</t>
+  </si>
+  <si>
+    <t>Test@%^$%^%^&amp;%^^%^&amp;^%^&amp;%^dhgf</t>
+  </si>
+  <si>
+    <t>Test_dhgf__c</t>
+  </si>
+  <si>
+    <t>Test N1</t>
+  </si>
+  <si>
+    <t>Test Na2</t>
+  </si>
+  <si>
+    <t>Test Nav3</t>
+  </si>
+  <si>
+    <t>Test Nava4</t>
+  </si>
+  <si>
+    <t>Test Navat5</t>
+  </si>
+  <si>
+    <t>Test Navata6</t>
+  </si>
+  <si>
+    <t>Test Navatar7</t>
+  </si>
+  <si>
+    <t>LastModifiedBy.UserRole.Name</t>
+  </si>
+  <si>
+    <t>DT-0019</t>
+  </si>
+  <si>
+    <t>DT-0020</t>
+  </si>
+  <si>
+    <t>DT-0021</t>
+  </si>
+  <si>
+    <t>DT-0022</t>
+  </si>
+  <si>
+    <t>DT-0023</t>
+  </si>
+  <si>
+    <t>DT-0024</t>
+  </si>
+  <si>
+    <t>DT-0025</t>
+  </si>
+  <si>
+    <t>DT-0026</t>
+  </si>
+  <si>
+    <t>DT-0027</t>
+  </si>
+  <si>
+    <t>DT-0028</t>
+  </si>
+  <si>
+    <t>DT-0029</t>
+  </si>
+  <si>
+    <t>Module3Tc050_CreateNewItemTaskOnNavigationTab</t>
+  </si>
+  <si>
+    <t>Module3Tc051_CreateNewItemsOnNavigationPage</t>
+  </si>
+  <si>
+    <t>Create New,70,,,,,,&lt;break&gt;Account,5,Create New,Account,,,,&lt;break&gt;Fund,10,Create New,navpeII__Fund__c,,,,&lt;break&gt;Task,15,Create New,Task,,,</t>
+  </si>
+  <si>
+    <t>Module3Tc055_MakeParentItemAsChildOfOtherItem</t>
+  </si>
+  <si>
+    <t>Create New</t>
+  </si>
+  <si>
+    <t>Module3Tc054_CreateRecordsAfterNavigationThroughNavigationMenu</t>
+  </si>
+  <si>
+    <t>Create New/Account&lt;break&gt;Create New/Fund&lt;break&gt;Create New/Task</t>
+  </si>
+  <si>
+    <t>Module3Tc057_DeleteCreateNewItemFromNavigationPage</t>
+  </si>
+  <si>
+    <t>Create New&lt;break&gt;Account&lt;break&gt;Fund&lt;break&gt;Task</t>
+  </si>
+  <si>
+    <t>Module3Tc058_Create20ItemsUnderAParentItemAndVerfiyNavigationMenu</t>
+  </si>
+  <si>
+    <t>Child1&lt;break&gt;Child2&lt;break&gt;Child3&lt;break&gt;Child4&lt;break&gt;Child5&lt;break&gt;Child6&lt;break&gt;Child7&lt;break&gt;Child8&lt;break&gt;Child9&lt;break&gt;Child10&lt;break&gt;Child11&lt;break&gt;Child12&lt;break&gt;Child13&lt;break&gt;Child14&lt;break&gt;Child15&lt;break&gt;Child16&lt;break&gt;Child17&lt;break&gt;Child18&lt;break&gt;Child19&lt;break&gt;Child20</t>
+  </si>
+  <si>
+    <t>AllParent</t>
   </si>
 </sst>
 </file>
@@ -1275,7 +1580,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1325,6 +1630,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF080707"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1371,7 +1682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1423,6 +1734,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1704,7 +2016,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1720,9 +2032,10 @@
     <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="66" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>318</v>
       </c>
@@ -1742,19 +2055,22 @@
         <v>338</v>
       </c>
       <c r="G1" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>387</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>388</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>389</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="13" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>323</v>
       </c>
@@ -1765,7 +2081,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>326</v>
       </c>
@@ -1776,7 +2092,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>329</v>
       </c>
@@ -1787,7 +2103,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>339</v>
       </c>
@@ -1795,7 +2111,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>341</v>
       </c>
@@ -1806,7 +2122,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>344</v>
       </c>
@@ -1814,105 +2130,234 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B8" t="s">
         <v>324</v>
       </c>
       <c r="G8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="B9" t="s">
         <v>392</v>
       </c>
-      <c r="B9" t="s">
+      <c r="H9" t="s">
         <v>393</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>394</v>
       </c>
-      <c r="I9" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="B10" t="s">
         <v>396</v>
       </c>
-      <c r="B10" t="s">
+      <c r="G10" t="s">
         <v>397</v>
       </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="B11" t="s">
         <v>399</v>
       </c>
-      <c r="B11" t="s">
+      <c r="J11" t="s">
         <v>400</v>
       </c>
-      <c r="J11" t="s">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="B12" t="s">
+        <v>399</v>
+      </c>
+      <c r="J12" t="s">
         <v>402</v>
       </c>
-      <c r="B12" t="s">
-        <v>400</v>
-      </c>
-      <c r="J12" t="s">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="B13" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="B13" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="B14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="B14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="B15" t="s">
+        <v>399</v>
+      </c>
+      <c r="H15" t="s">
+        <v>466</v>
+      </c>
+      <c r="I15" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>406</v>
       </c>
-      <c r="B15" t="s">
-        <v>400</v>
-      </c>
-      <c r="I15" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="B16" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="B16" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>408</v>
-      </c>
       <c r="B17" t="s">
-        <v>400</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="B18" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>468</v>
+      </c>
+      <c r="B19" t="s">
+        <v>399</v>
+      </c>
+      <c r="H19" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="B20" t="s">
+        <v>470</v>
+      </c>
+      <c r="H20" t="s">
+        <v>471</v>
+      </c>
+      <c r="I20" t="s">
+        <v>394</v>
+      </c>
+      <c r="J20" t="s">
+        <v>472</v>
+      </c>
+      <c r="K20" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="B21" t="s">
+        <v>470</v>
+      </c>
+      <c r="K21" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>474</v>
+      </c>
+      <c r="B22" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="B23" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>498</v>
+      </c>
+      <c r="B24" t="s">
+        <v>362</v>
+      </c>
+      <c r="E24">
+        <v>35</v>
+      </c>
+      <c r="K24" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="B25" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B26" t="s">
+        <v>470</v>
+      </c>
+      <c r="F26" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="B27" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="B28" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>507</v>
+      </c>
+      <c r="B29" t="s">
+        <v>508</v>
+      </c>
+      <c r="F29" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>
@@ -1931,13 +2376,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2027,20 +2472,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2092,6 +2537,20 @@
       </c>
       <c r="E3" s="5" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" t="s">
+        <v>436</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E4" t="s">
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -2295,8 +2754,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,15 +2859,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -2537,16 +2996,16 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2571,184 +3030,502 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B2" t="s">
         <v>358</v>
       </c>
-      <c r="C2" t="s">
-        <v>358</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B3" t="s">
         <v>359</v>
       </c>
-      <c r="C3" t="s">
-        <v>359</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B4" t="s">
         <v>360</v>
       </c>
-      <c r="C4" t="s">
-        <v>360</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B6" t="s">
         <v>361</v>
       </c>
-      <c r="C6" t="s">
-        <v>362</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B7" t="s">
-        <v>363</v>
-      </c>
-      <c r="C7" t="s">
-        <v>363</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B8" t="s">
-        <v>358</v>
-      </c>
-      <c r="C8" t="s">
-        <v>358</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9" t="s">
-        <v>360</v>
-      </c>
-      <c r="C9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>381</v>
-      </c>
-      <c r="B10" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" t="s">
-        <v>382</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
+        <v>380</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B11" t="s">
-        <v>364</v>
-      </c>
-      <c r="C11" t="s">
-        <v>358</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B12" t="s">
-        <v>365</v>
-      </c>
-      <c r="C12" t="s">
-        <v>359</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
+        <v>364</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13" t="s">
-        <v>366</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>367</v>
       </c>
-      <c r="C14" t="s">
-        <v>368</v>
-      </c>
-      <c r="D14">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3" t="s">
+        <v>436</v>
+      </c>
+      <c r="E3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B4" t="s">
+        <v>434</v>
+      </c>
+      <c r="C4" t="s">
+        <v>435</v>
+      </c>
+      <c r="D4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>440</v>
+      </c>
+      <c r="B5" t="s">
+        <v>434</v>
+      </c>
+      <c r="C5" t="s">
+        <v>435</v>
+      </c>
+      <c r="D5" t="s">
+        <v>436</v>
+      </c>
+      <c r="E5" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>441</v>
+      </c>
+      <c r="B6" t="s">
+        <v>434</v>
+      </c>
+      <c r="C6" t="s">
+        <v>435</v>
+      </c>
+      <c r="D6" t="s">
+        <v>436</v>
+      </c>
+      <c r="E6" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7" t="s">
+        <v>434</v>
+      </c>
+      <c r="C7" t="s">
+        <v>435</v>
+      </c>
+      <c r="D7" t="s">
+        <v>436</v>
+      </c>
+      <c r="E7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>446</v>
+      </c>
+      <c r="B2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E2" t="s">
+        <v>447</v>
+      </c>
+      <c r="F2" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>449</v>
+      </c>
+      <c r="B3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" t="s">
+        <v>434</v>
+      </c>
+      <c r="E3" t="s">
+        <v>450</v>
+      </c>
+      <c r="F3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" t="s">
+        <v>434</v>
+      </c>
+      <c r="E4" t="s">
+        <v>452</v>
+      </c>
+      <c r="F4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>453</v>
+      </c>
+      <c r="B5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" t="s">
+        <v>428</v>
+      </c>
+      <c r="D5" t="s">
+        <v>434</v>
+      </c>
+      <c r="E5" t="s">
+        <v>447</v>
+      </c>
+      <c r="F5" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>454</v>
+      </c>
+      <c r="B6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C6" t="s">
+        <v>428</v>
+      </c>
+      <c r="D6" t="s">
+        <v>434</v>
+      </c>
+      <c r="E6" t="s">
+        <v>450</v>
+      </c>
+      <c r="F6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>455</v>
+      </c>
+      <c r="B7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C7" t="s">
+        <v>428</v>
+      </c>
+      <c r="D7" t="s">
+        <v>434</v>
+      </c>
+      <c r="E7" t="s">
+        <v>452</v>
+      </c>
+      <c r="F7" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>456</v>
+      </c>
+      <c r="B8" t="s">
+        <v>493</v>
+      </c>
+      <c r="C8" t="s">
+        <v>428</v>
+      </c>
+      <c r="D8" t="s">
+        <v>434</v>
+      </c>
+      <c r="E8" t="s">
+        <v>447</v>
+      </c>
+      <c r="F8" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>457</v>
+      </c>
+      <c r="B9" t="s">
+        <v>494</v>
+      </c>
+      <c r="C9" t="s">
+        <v>428</v>
+      </c>
+      <c r="D9" t="s">
+        <v>434</v>
+      </c>
+      <c r="E9" t="s">
+        <v>450</v>
+      </c>
+      <c r="F9" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>458</v>
+      </c>
+      <c r="B10" t="s">
+        <v>495</v>
+      </c>
+      <c r="C10" t="s">
+        <v>428</v>
+      </c>
+      <c r="D10" t="s">
+        <v>434</v>
+      </c>
+      <c r="E10" t="s">
+        <v>452</v>
+      </c>
+      <c r="F10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>459</v>
+      </c>
+      <c r="B11" t="s">
+        <v>496</v>
+      </c>
+      <c r="C11" t="s">
+        <v>428</v>
+      </c>
+      <c r="D11" t="s">
+        <v>434</v>
+      </c>
+      <c r="E11" t="s">
+        <v>447</v>
+      </c>
+      <c r="F11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>460</v>
+      </c>
+      <c r="B12" t="s">
+        <v>497</v>
+      </c>
+      <c r="C12" t="s">
+        <v>428</v>
+      </c>
+      <c r="D12" t="s">
+        <v>434</v>
+      </c>
+      <c r="E12" t="s">
+        <v>450</v>
+      </c>
+      <c r="F12" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -2856,10 +3633,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2872,7 +3649,7 @@
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -2891,8 +3668,11 @@
       <c r="F1" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2912,7 +3692,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>199</v>
       </c>
@@ -2929,7 +3709,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>202</v>
       </c>
@@ -2946,7 +3726,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -2963,7 +3743,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>206</v>
       </c>
@@ -2980,7 +3760,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>208</v>
       </c>
@@ -2997,7 +3777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3014,7 +3794,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>212</v>
       </c>
@@ -3031,7 +3811,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>214</v>
       </c>
@@ -3048,7 +3828,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>216</v>
       </c>
@@ -3065,7 +3845,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>218</v>
       </c>
@@ -3082,7 +3862,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>230</v>
       </c>
@@ -3099,7 +3879,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>231</v>
       </c>
@@ -3116,7 +3896,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>232</v>
       </c>
@@ -3133,7 +3913,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -3420,6 +4200,26 @@
       </c>
       <c r="F32" s="8" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>476</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" t="s">
+        <v>477</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G33" t="s">
+        <v>478</v>
       </c>
     </row>
   </sheetData>
@@ -3430,10 +4230,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO23"/>
+  <dimension ref="A1:ALO26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,7 +4241,7 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -4651,6 +5451,28 @@
         <v>301</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>462</v>
+      </c>
+      <c r="B25" t="s">
+        <v>409</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>463</v>
+      </c>
+      <c r="B26" t="s">
+        <v>464</v>
+      </c>
+      <c r="C26" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4658,10 +5480,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR12"/>
+  <dimension ref="A1:ALR20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5852,6 +6674,200 @@
         <v>299</v>
       </c>
     </row>
+    <row r="14" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>408</v>
+      </c>
+      <c r="B14" t="s">
+        <v>479</v>
+      </c>
+      <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
+        <v>409</v>
+      </c>
+      <c r="E14" t="s">
+        <v>410</v>
+      </c>
+      <c r="F14">
+        <v>8435985993</v>
+      </c>
+      <c r="H14" t="s">
+        <v>411</v>
+      </c>
+      <c r="I14" t="s">
+        <v>412</v>
+      </c>
+      <c r="J14" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>414</v>
+      </c>
+      <c r="B15" t="s">
+        <v>480</v>
+      </c>
+      <c r="C15" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" t="s">
+        <v>409</v>
+      </c>
+      <c r="E15" t="s">
+        <v>415</v>
+      </c>
+      <c r="F15">
+        <v>8435985993</v>
+      </c>
+      <c r="H15" t="s">
+        <v>416</v>
+      </c>
+      <c r="I15" t="s">
+        <v>412</v>
+      </c>
+      <c r="J15" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>417</v>
+      </c>
+      <c r="B16" t="s">
+        <v>481</v>
+      </c>
+      <c r="C16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>409</v>
+      </c>
+      <c r="E16" t="s">
+        <v>418</v>
+      </c>
+      <c r="F16">
+        <v>8435985993</v>
+      </c>
+      <c r="H16" t="s">
+        <v>411</v>
+      </c>
+      <c r="I16" t="s">
+        <v>412</v>
+      </c>
+      <c r="J16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>419</v>
+      </c>
+      <c r="B17" t="s">
+        <v>482</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
+        <v>409</v>
+      </c>
+      <c r="E17" t="s">
+        <v>420</v>
+      </c>
+      <c r="F17">
+        <v>8435985993</v>
+      </c>
+      <c r="H17" t="s">
+        <v>416</v>
+      </c>
+      <c r="I17" t="s">
+        <v>412</v>
+      </c>
+      <c r="J17" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>421</v>
+      </c>
+      <c r="B18" t="s">
+        <v>483</v>
+      </c>
+      <c r="C18" t="s">
+        <v>422</v>
+      </c>
+      <c r="D18" t="s">
+        <v>409</v>
+      </c>
+      <c r="F18">
+        <v>8435985993</v>
+      </c>
+      <c r="H18" t="s">
+        <v>411</v>
+      </c>
+      <c r="I18" t="s">
+        <v>412</v>
+      </c>
+      <c r="J18" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B19" t="s">
+        <v>484</v>
+      </c>
+      <c r="C19" t="s">
+        <v>424</v>
+      </c>
+      <c r="D19" t="s">
+        <v>409</v>
+      </c>
+      <c r="F19">
+        <v>8435985993</v>
+      </c>
+      <c r="H19" t="s">
+        <v>416</v>
+      </c>
+      <c r="I19" t="s">
+        <v>412</v>
+      </c>
+      <c r="J19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>425</v>
+      </c>
+      <c r="B20" t="s">
+        <v>485</v>
+      </c>
+      <c r="C20" t="s">
+        <v>426</v>
+      </c>
+      <c r="D20" t="s">
+        <v>409</v>
+      </c>
+      <c r="F20">
+        <v>8435985993</v>
+      </c>
+      <c r="H20" t="s">
+        <v>411</v>
+      </c>
+      <c r="I20" t="s">
+        <v>412</v>
+      </c>
+      <c r="J20" t="s">
+        <v>413</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5970,10 +6986,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML14"/>
+  <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7188,6 +8204,20 @@
         <v>286</v>
       </c>
     </row>
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>427</v>
+      </c>
+      <c r="B16" t="s">
+        <v>428</v>
+      </c>
+      <c r="C16" t="s">
+        <v>409</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7204,10 +8234,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7269,15 +8299,15 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -7347,19 +8377,19 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>385</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel for Module 3 tc061-072
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -30,6 +30,7 @@
     <sheet name="Fields" sheetId="19" r:id="rId16"/>
     <sheet name="Attendees" sheetId="20" r:id="rId17"/>
     <sheet name="Deal Team" sheetId="21" r:id="rId18"/>
+    <sheet name="Coverages" sheetId="22" r:id="rId19"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="531">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1571,6 +1572,69 @@
   </si>
   <si>
     <t>AllParent</t>
+  </si>
+  <si>
+    <t>M4Att7</t>
+  </si>
+  <si>
+    <t>M4Att8</t>
+  </si>
+  <si>
+    <t>M4Att9</t>
+  </si>
+  <si>
+    <t>Module3Tc063_2_RemoveTheRecordCreationRightForStandardUser</t>
+  </si>
+  <si>
+    <t>Module3Tc065_CreateMyIndustryMenuItem</t>
+  </si>
+  <si>
+    <t>My Industry</t>
+  </si>
+  <si>
+    <t>/lightning/cmp/c__RedirectCmp?c__coverage=industry</t>
+  </si>
+  <si>
+    <t>Coverage_Name</t>
+  </si>
+  <si>
+    <t>Coverage1</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Coverage2</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Coverage3</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Coverage4</t>
+  </si>
+  <si>
+    <t>Business Services</t>
+  </si>
+  <si>
+    <t>Coverage5</t>
+  </si>
+  <si>
+    <t>Coverage6</t>
+  </si>
+  <si>
+    <t>Pharma</t>
+  </si>
+  <si>
+    <t>M4tc016_UpdateImageOnUserProfile</t>
   </si>
 </sst>
 </file>
@@ -2016,11 +2080,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2035,7 +2097,7 @@
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>318</v>
       </c>
@@ -2069,8 +2131,11 @@
       <c r="K1" s="13" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>323</v>
       </c>
@@ -2081,7 +2146,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>326</v>
       </c>
@@ -2092,7 +2157,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>329</v>
       </c>
@@ -2103,7 +2168,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>339</v>
       </c>
@@ -2111,7 +2176,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>341</v>
       </c>
@@ -2122,7 +2187,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>344</v>
       </c>
@@ -2130,7 +2195,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>389</v>
       </c>
@@ -2141,7 +2206,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>391</v>
       </c>
@@ -2155,7 +2220,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>395</v>
       </c>
@@ -2166,7 +2231,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>398</v>
       </c>
@@ -2177,7 +2242,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>401</v>
       </c>
@@ -2188,7 +2253,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>403</v>
       </c>
@@ -2196,7 +2261,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>404</v>
       </c>
@@ -2204,7 +2269,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>405</v>
       </c>
@@ -2218,7 +2283,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>406</v>
       </c>
@@ -2226,7 +2291,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>407</v>
       </c>
@@ -2234,7 +2299,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>467</v>
       </c>
@@ -2242,7 +2307,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>468</v>
       </c>
@@ -2253,7 +2318,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>469</v>
       </c>
@@ -2273,7 +2338,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>473</v>
       </c>
@@ -2284,7 +2349,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>474</v>
       </c>
@@ -2292,7 +2357,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>475</v>
       </c>
@@ -2300,7 +2365,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>498</v>
       </c>
@@ -2314,7 +2379,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>499</v>
       </c>
@@ -2322,7 +2387,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>501</v>
       </c>
@@ -2333,7 +2398,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>503</v>
       </c>
@@ -2341,7 +2406,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>505</v>
       </c>
@@ -2349,7 +2414,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>507</v>
       </c>
@@ -2360,9 +2425,39 @@
         <v>509</v>
       </c>
     </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="B30" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>514</v>
+      </c>
+      <c r="B31" t="s">
+        <v>515</v>
+      </c>
+      <c r="E31">
+        <v>-20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>530</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3142,9 +3237,11 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3268,6 +3365,57 @@
         <v>436</v>
       </c>
       <c r="E7" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>510</v>
+      </c>
+      <c r="B8" t="s">
+        <v>434</v>
+      </c>
+      <c r="C8" t="s">
+        <v>435</v>
+      </c>
+      <c r="D8" t="s">
+        <v>436</v>
+      </c>
+      <c r="E8" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" t="s">
+        <v>434</v>
+      </c>
+      <c r="C9" t="s">
+        <v>435</v>
+      </c>
+      <c r="D9" t="s">
+        <v>436</v>
+      </c>
+      <c r="E9" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>512</v>
+      </c>
+      <c r="B10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C10" t="s">
+        <v>435</v>
+      </c>
+      <c r="D10" t="s">
+        <v>436</v>
+      </c>
+      <c r="E10" t="s">
         <v>437</v>
       </c>
     </row>
@@ -3526,6 +3674,103 @@
       </c>
       <c r="F12" t="s">
         <v>448</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" t="s">
+        <v>519</v>
+      </c>
+      <c r="C2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B3" t="s">
+        <v>522</v>
+      </c>
+      <c r="C3" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>523</v>
+      </c>
+      <c r="B4" t="s">
+        <v>524</v>
+      </c>
+      <c r="C4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>525</v>
+      </c>
+      <c r="B5" t="s">
+        <v>526</v>
+      </c>
+      <c r="C5" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>527</v>
+      </c>
+      <c r="B6" t="s">
+        <v>413</v>
+      </c>
+      <c r="C6" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>528</v>
+      </c>
+      <c r="B7" t="s">
+        <v>529</v>
+      </c>
+      <c r="C7" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel Updated for Module 5 Toggle
Signed-off-by: azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azhar Alam\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABCB675-372F-45ED-92DB-02525DA4C03E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="542">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -491,24 +492,15 @@
     <t>TOGGLEINS1</t>
   </si>
   <si>
-    <t>Alexa Info</t>
-  </si>
-  <si>
     <t>TOGGLEFUND1</t>
   </si>
   <si>
-    <t>Alexa Fund</t>
-  </si>
-  <si>
     <t>TOGGLEFUND2</t>
   </si>
   <si>
     <t>TOGGLEDEAL1</t>
   </si>
   <si>
-    <t>Alexa Sep Deal 2020</t>
-  </si>
-  <si>
     <t>SDG_Name</t>
   </si>
   <si>
@@ -521,9 +513,6 @@
     <t>TOGGLESDG1</t>
   </si>
   <si>
-    <t>Custom SDG</t>
-  </si>
-  <si>
     <t>navpeII__Pipeline__c</t>
   </si>
   <si>
@@ -542,9 +531,6 @@
     <t>RT</t>
   </si>
   <si>
-    <t>12/22/2020</t>
-  </si>
-  <si>
     <t>IT Related</t>
   </si>
   <si>
@@ -554,9 +540,6 @@
     <t>CLOSEDQA1</t>
   </si>
   <si>
-    <t>12/7/2020</t>
-  </si>
-  <si>
     <t>Finance Related</t>
   </si>
   <si>
@@ -572,9 +555,6 @@
     <t>TOGGLEME1</t>
   </si>
   <si>
-    <t>Alexa Event 1</t>
-  </si>
-  <si>
     <t>Third Party Event</t>
   </si>
   <si>
@@ -1635,12 +1615,66 @@
   </si>
   <si>
     <t>M4tc016_UpdateImageOnUserProfile</t>
+  </si>
+  <si>
+    <t>M5Alexa Info</t>
+  </si>
+  <si>
+    <t>TOGGLELP1</t>
+  </si>
+  <si>
+    <t>M5Alexa Limited partner</t>
+  </si>
+  <si>
+    <t>TOGGLEPS1</t>
+  </si>
+  <si>
+    <t>M5Alexa Fund Partnership</t>
+  </si>
+  <si>
+    <t>TOGGLEPS2</t>
+  </si>
+  <si>
+    <t>M5Alexa Co-Invest Partnership</t>
+  </si>
+  <si>
+    <t>TOGGLECMT1</t>
+  </si>
+  <si>
+    <t>TOGGLECMT2</t>
+  </si>
+  <si>
+    <t>M5Alexa Fund</t>
+  </si>
+  <si>
+    <t>M5Alexa Co-Invest Fund</t>
+  </si>
+  <si>
+    <t>M5Alexa Sep Deal 2020</t>
+  </si>
+  <si>
+    <t>3/7/2021</t>
+  </si>
+  <si>
+    <t>3/4/2021</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>M5Custom SDG</t>
+  </si>
+  <si>
+    <t>M5Alexa Event 1</t>
+  </si>
+  <si>
+    <t>3/9/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -1802,7 +1836,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2079,10 +2113,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2099,362 +2133,362 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="J1" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="L1" s="13" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B3" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D3" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="E4" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B6" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="F6" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B7" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B8" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G8" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B9" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="H9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="I9" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B10" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G10" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="B11" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="J11" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B12" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="J12" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B13" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B14" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B15" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="H15" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="I15" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B16" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B17" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="B18" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="B19" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="H19" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="B20" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="H20" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="I20" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="J20" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="K20" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="B21" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="K21" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="B22" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="B23" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B24" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E24">
         <v>35</v>
       </c>
       <c r="K24" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B25" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B26" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="F26" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="B27" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="B28" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="B29" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="F29" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="B30" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="B31" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="E31">
         <v>-20</v>
       </c>
       <c r="L31" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M"/>
+    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2462,11 +2496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,79 +2519,79 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>149</v>
+        <v>524</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>154</v>
+        <v>535</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>176</v>
+        <v>540</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2566,11 +2600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,47 +2622,47 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>176</v>
+        <v>540</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>178</v>
+        <v>170</v>
+      </c>
+      <c r="D2" t="s">
+        <v>541</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>149</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>52</v>
@@ -2636,16 +2670,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="B4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -2655,7 +2689,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2712,7 +2746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2842,7 +2876,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2945,7 +2979,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2970,54 +3004,54 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C2" t="s">
         <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="H2" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="I2" t="s">
         <v>35</v>
@@ -3025,60 +3059,60 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D3" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="H3" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="I3" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F4" t="s">
         <v>310</v>
       </c>
-      <c r="E4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4" t="s">
-        <v>317</v>
-      </c>
       <c r="G4" s="28" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="H4" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="I4" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -3087,7 +3121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3108,48 +3142,48 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B3" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -3157,77 +3191,77 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="B6" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="B7" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B8" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B11" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B12" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B13" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -3236,7 +3270,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3254,169 +3288,169 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D2" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E2" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="B3" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C3" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D3" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E3" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E4" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B5" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C5" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D5" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E5" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C6" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E6" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="B7" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C7" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D7" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E7" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="B8" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C8" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D8" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E8" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="B9" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C9" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D9" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E9" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="B10" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C10" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D10" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E10" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3425,7 +3459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3441,239 +3475,239 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E2" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F2" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="B3" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="C3" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D3" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E3" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="F3" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="C4" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D4" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E4" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="F4" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="B5" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="C5" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E5" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F5" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="B6" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="C6" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D6" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E6" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="F6" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="C7" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D7" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E7" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="F7" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="B8" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="C8" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D8" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E8" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F8" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="B9" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="C9" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D9" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E9" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="F9" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="B10" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="C10" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D10" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E10" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="F10" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="B11" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="C11" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D11" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E11" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="F11" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="B12" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="C12" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="D12" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E12" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="F12" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3682,7 +3716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3701,7 +3735,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
@@ -3709,68 +3743,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="B2" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="C2" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="B3" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="C3" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="B4" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="C4" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="B5" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="C5" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="B6" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C6" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="B7" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="C7" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -3779,7 +3813,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3877,7 +3911,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3914,7 +3948,7 @@
         <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -3939,16 +3973,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
         <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>43</v>
@@ -3956,16 +3990,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>43</v>
@@ -3973,16 +4007,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>43</v>
@@ -3990,16 +4024,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>43</v>
@@ -4007,16 +4041,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
         <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>43</v>
@@ -4024,16 +4058,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="B8" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>43</v>
@@ -4041,16 +4075,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>43</v>
@@ -4058,16 +4092,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B10" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
         <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>43</v>
@@ -4075,16 +4109,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>43</v>
@@ -4092,16 +4126,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>43</v>
@@ -4109,7 +4143,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -4118,7 +4152,7 @@
         <v>46</v>
       </c>
       <c r="D13" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>43</v>
@@ -4126,7 +4160,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -4135,7 +4169,7 @@
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>43</v>
@@ -4143,7 +4177,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -4152,7 +4186,7 @@
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>43</v>
@@ -4160,7 +4194,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -4169,7 +4203,7 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>43</v>
@@ -4177,7 +4211,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -4186,7 +4220,7 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>43</v>
@@ -4194,7 +4228,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -4203,7 +4237,7 @@
         <v>46</v>
       </c>
       <c r="D18" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>43</v>
@@ -4211,7 +4245,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -4220,7 +4254,7 @@
         <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>43</v>
@@ -4228,7 +4262,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -4237,7 +4271,7 @@
         <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>43</v>
@@ -4245,7 +4279,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -4254,7 +4288,7 @@
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>43</v>
@@ -4262,7 +4296,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -4271,7 +4305,7 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>43</v>
@@ -4279,16 +4313,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C23" t="s">
         <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>43</v>
@@ -4296,16 +4330,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B24" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C24" t="s">
         <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>43</v>
@@ -4313,16 +4347,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B25" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>43</v>
@@ -4330,16 +4364,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B26" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C26" t="s">
         <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>43</v>
@@ -4347,16 +4381,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B27" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C27" t="s">
         <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>43</v>
@@ -4364,16 +4398,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C28" t="s">
         <v>46</v>
       </c>
       <c r="D28" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>43</v>
@@ -4381,16 +4415,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C29" t="s">
         <v>46</v>
       </c>
       <c r="D29" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>43</v>
@@ -4398,16 +4432,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C30" t="s">
         <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>43</v>
@@ -4415,16 +4449,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C31" t="s">
         <v>46</v>
       </c>
       <c r="D31" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>43</v>
@@ -4432,16 +4466,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B32" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C32" t="s">
         <v>46</v>
       </c>
       <c r="D32" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>43</v>
@@ -4449,7 +4483,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
@@ -4458,13 +4492,13 @@
         <v>46</v>
       </c>
       <c r="D33" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>43</v>
       </c>
       <c r="G33" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -4474,11 +4508,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:ALO31"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5621,10 +5655,10 @@
     </row>
     <row r="13" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>81</v>
@@ -5635,87 +5669,128 @@
         <v>148</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>149</v>
+        <v>524</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>35</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>525</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>526</v>
+      </c>
+      <c r="C18" s="25"/>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>300</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>301</v>
-      </c>
+      <c r="A19" s="23" t="s">
+        <v>527</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>528</v>
+      </c>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>302</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>301</v>
-      </c>
+      <c r="A20" s="23" t="s">
+        <v>529</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>530</v>
+      </c>
+      <c r="C20" s="25"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>303</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
+      <c r="A21" s="23" t="s">
+        <v>531</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="25"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>304</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>298</v>
-      </c>
-      <c r="C22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>305</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>301</v>
+      <c r="A22" s="23" t="s">
+        <v>532</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="25"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>293</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" s="22" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>462</v>
-      </c>
-      <c r="B25" t="s">
-        <v>409</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
+        <v>295</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>272</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>463</v>
-      </c>
-      <c r="B26" t="s">
-        <v>464</v>
+        <v>296</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>264</v>
       </c>
       <c r="C26" t="s">
-        <v>301</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>298</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C28" s="22" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>455</v>
+      </c>
+      <c r="B30" t="s">
+        <v>402</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>456</v>
+      </c>
+      <c r="B31" t="s">
+        <v>457</v>
+      </c>
+      <c r="C31" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -5724,7 +5799,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:ALR20"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -6870,247 +6945,247 @@
     </row>
     <row r="10" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B10" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C10" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="E10" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="11" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="B11" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E11" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C12" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D12" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="14" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B14" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="C14" t="s">
         <v>111</v>
       </c>
       <c r="D14" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E14" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="F14">
         <v>8435985993</v>
       </c>
       <c r="H14" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="I14" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J14" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B15" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="C15" t="s">
         <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E15" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="F15">
         <v>8435985993</v>
       </c>
       <c r="H15" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="I15" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J15" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B16" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
       </c>
       <c r="D16" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E16" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="F16">
         <v>8435985993</v>
       </c>
       <c r="H16" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="I16" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J16" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B17" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="C17" t="s">
         <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E17" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="F17">
         <v>8435985993</v>
       </c>
       <c r="H17" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="I17" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J17" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B18" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="C18" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="D18" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F18">
         <v>8435985993</v>
       </c>
       <c r="H18" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="I18" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J18" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B19" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="C19" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="D19" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F19">
         <v>8435985993</v>
       </c>
       <c r="H19" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="I19" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J19" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B20" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C20" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="D20" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="F20">
         <v>8435985993</v>
       </c>
       <c r="H20" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="I20" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="J20" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -7119,11 +7194,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A7" sqref="A7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7198,10 +7273,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>151</v>
+        <v>533</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>62</v>
@@ -7212,10 +7287,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>64</v>
+        <v>534</v>
       </c>
       <c r="C8" s="25" t="s">
         <v>62</v>
@@ -7230,11 +7305,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8311,10 +8386,10 @@
     </row>
     <row r="3" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
@@ -8325,10 +8400,10 @@
     </row>
     <row r="4" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B4" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C4" t="s">
         <v>52</v>
@@ -8339,10 +8414,10 @@
     </row>
     <row r="7" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>154</v>
+        <v>535</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="24" t="s">
@@ -8351,113 +8426,113 @@
     </row>
     <row r="10" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B10" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C10" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D10" t="s">
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="F11" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12" t="s">
         <v>271</v>
       </c>
-      <c r="D12" t="s">
-        <v>278</v>
-      </c>
       <c r="E12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>272</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C13" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D13" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E13" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C14" t="s">
+        <v>264</v>
+      </c>
+      <c r="D14" t="s">
         <v>271</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>278</v>
       </c>
-      <c r="E14" t="s">
-        <v>285</v>
-      </c>
       <c r="F14" s="22" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="B16" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C16" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -8470,11 +8545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8490,13 +8565,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>98</v>
@@ -8504,33 +8579,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>166</v>
+        <v>161</v>
+      </c>
+      <c r="C2" t="s">
+        <v>536</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C3" t="s">
+        <v>537</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>171</v>
+      <c r="E3" s="5" t="s">
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -8540,11 +8618,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8560,35 +8638,35 @@
         <v>9</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>539</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>159</v>
+        <v>539</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -8600,41 +8678,41 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Excel for M3 tc073-080
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azhar Alam\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABCB675-372F-45ED-92DB-02525DA4C03E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="552">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1669,12 +1668,42 @@
   </si>
   <si>
     <t>3/9/2021</t>
+  </si>
+  <si>
+    <t>M4tc028_VerifyBrokenImageInContactProfile</t>
+  </si>
+  <si>
+    <t>JPEGImage</t>
+  </si>
+  <si>
+    <t>https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>M4CON8</t>
+  </si>
+  <si>
+    <t>Test Navatar8</t>
+  </si>
+  <si>
+    <t>Contact8</t>
+  </si>
+  <si>
+    <t>Module3Tc074_CreateMyRegionMenuItem</t>
+  </si>
+  <si>
+    <t>My Region</t>
+  </si>
+  <si>
+    <t>/lightning/cmp/c__RedirectCmp?c__coverage=Region</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -1836,7 +1865,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2113,10 +2142,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2131,7 +2162,7 @@
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>311</v>
       </c>
@@ -2168,8 +2199,11 @@
       <c r="L1" s="13" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="13" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>316</v>
       </c>
@@ -2180,7 +2214,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>319</v>
       </c>
@@ -2191,7 +2225,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>322</v>
       </c>
@@ -2202,7 +2236,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>332</v>
       </c>
@@ -2210,7 +2244,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>334</v>
       </c>
@@ -2221,7 +2255,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>337</v>
       </c>
@@ -2229,7 +2263,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>382</v>
       </c>
@@ -2240,7 +2274,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>384</v>
       </c>
@@ -2254,7 +2288,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>388</v>
       </c>
@@ -2265,7 +2299,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>391</v>
       </c>
@@ -2276,7 +2310,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>394</v>
       </c>
@@ -2287,7 +2321,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>396</v>
       </c>
@@ -2295,7 +2329,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>397</v>
       </c>
@@ -2303,7 +2337,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>398</v>
       </c>
@@ -2317,7 +2351,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>399</v>
       </c>
@@ -2483,20 +2517,46 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
+        <v>549</v>
+      </c>
+      <c r="B32" t="s">
+        <v>550</v>
+      </c>
+      <c r="E32">
+        <v>-25</v>
+      </c>
+      <c r="L32" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
         <v>523</v>
+      </c>
+      <c r="L33" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>542</v>
+      </c>
+      <c r="M34" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L30" r:id="rId1" display="https://pe4604--c.documentforce.com/profilephoto/7294x000000I280/M"/>
+    <hyperlink ref="L33" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2600,11 +2660,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2689,7 +2749,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2746,7 +2806,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2876,7 +2936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2979,7 +3039,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3121,7 +3181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3270,7 +3330,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3459,7 +3519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3716,7 +3776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3813,7 +3873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3911,10 +3971,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -4508,10 +4568,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -5799,11 +5859,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ALR20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR21"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7188,17 +7248,34 @@
         <v>406</v>
       </c>
     </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>546</v>
+      </c>
+      <c r="B21" t="s">
+        <v>547</v>
+      </c>
+      <c r="C21" t="s">
+        <v>548</v>
+      </c>
+      <c r="D21" t="s">
+        <v>402</v>
+      </c>
+      <c r="H21" t="s">
+        <v>409</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D8"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7305,11 +7382,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8545,7 +8622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8618,7 +8695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Added Module 3 TC001_2 add List view
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="661">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1981,6 +1981,51 @@
   </si>
   <si>
     <t>Create New&lt;break&gt;Account&lt;break&gt;Fund&lt;break&gt;Task1</t>
+  </si>
+  <si>
+    <t>Funds</t>
+  </si>
+  <si>
+    <t>M3Task1</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Call</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Test Comments for Log a call from Nav menu</t>
+  </si>
+  <si>
+    <t>M3Task2</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Multitagged Task 1</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Test Comments for New Task from Nav menu</t>
+  </si>
+  <si>
+    <t>M3Task3</t>
+  </si>
+  <si>
+    <t>New Meeting 1</t>
+  </si>
+  <si>
+    <t>Monday Morning Meeting</t>
+  </si>
+  <si>
+    <t>Test Comments for New Meeting from Nav menu</t>
   </si>
 </sst>
 </file>
@@ -3789,7 +3834,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3988,9 +4033,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3998,7 +4045,7 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4009,7 +4056,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>140</v>
       </c>
@@ -4018,7 +4065,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>138</v>
       </c>
@@ -4027,7 +4074,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>136</v>
       </c>
@@ -4036,7 +4083,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>134</v>
       </c>
@@ -4044,7 +4091,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>132</v>
       </c>
@@ -4052,7 +4099,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>130</v>
       </c>
@@ -4060,7 +4107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>128</v>
       </c>
@@ -4068,7 +4115,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>126</v>
       </c>
@@ -4076,12 +4123,90 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>124</v>
       </c>
       <c r="C10" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="13"/>
+    </row>
+    <row r="15" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
+        <v>647</v>
+      </c>
+      <c r="B15" s="50" t="s">
+        <v>648</v>
+      </c>
+      <c r="C15" s="50" t="s">
+        <v>649</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>650</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>652</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>653</v>
+      </c>
+      <c r="C16" s="50" t="s">
+        <v>654</v>
+      </c>
+      <c r="G16" s="50" t="s">
+        <v>655</v>
+      </c>
+      <c r="H16" s="50" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
+        <v>657</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>653</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>658</v>
+      </c>
+      <c r="F17" s="50" t="s">
+        <v>659</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>650</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -4990,7 +5115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -5755,8 +5880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALO49"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12701,79 +12826,85 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
       <c r="D2" s="39"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="39"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="11"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -12781,13 +12912,16 @@
         <v>582</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>646</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -12795,82 +12929,87 @@
         <v>583</v>
       </c>
       <c r="C5" t="s">
+        <v>646</v>
+      </c>
+      <c r="D5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
-      <c r="C7" s="22"/>
       <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="11"/>
+    </row>
+    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>610</v>
       </c>
       <c r="B9" s="50" t="s">
         <v>611</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>60</v>
-      </c>
       <c r="D9" s="22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="11"/>
+    </row>
+    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>147</v>
       </c>
       <c r="B12" s="50" t="s">
         <v>523</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>60</v>
-      </c>
       <c r="D12" s="22" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>148</v>
       </c>
       <c r="B13" s="50" t="s">
         <v>524</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="D13" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="E13" s="22" t="s">
         <v>93</v>
       </c>
     </row>
@@ -12884,7 +13023,7 @@
   <dimension ref="A1:AML19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A7:XFD9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Excel related to Module3
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="664">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2026,6 +2026,15 @@
   </si>
   <si>
     <t>Test Comments for New Meeting from Nav menu</t>
+  </si>
+  <si>
+    <t>Meeting_Type</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -4036,7 +4045,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4045,7 +4054,7 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4054,6 +4063,15 @@
       </c>
       <c r="C1" s="21" t="s">
         <v>141</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>661</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>662</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel updated for manual refrence Module 3 & Module 5
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sibaram\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akul Bhutani\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17370" windowHeight="6195" firstSheet="2" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Attendees" sheetId="20" r:id="rId18"/>
     <sheet name="Deal Team" sheetId="21" r:id="rId19"/>
     <sheet name="Coverages" sheetId="22" r:id="rId20"/>
+    <sheet name="SDGActions" sheetId="24" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1113" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="677">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1293,9 +1294,6 @@
     <t>LastModifiedBy.Email</t>
   </si>
   <si>
-    <t>LastModifiedBy.UserRoleId</t>
-  </si>
-  <si>
     <t>LastModifiedBy.UserRole.Nam</t>
   </si>
   <si>
@@ -2035,6 +2033,51 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Action_Order</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Event_Payload</t>
+  </si>
+  <si>
+    <t>Action_Type</t>
+  </si>
+  <si>
+    <t>SDGAction1</t>
+  </si>
+  <si>
+    <t>New Attendee</t>
+  </si>
+  <si>
+    <t>e.force:createRecord</t>
+  </si>
+  <si>
+    <t>{"entityApiName": "Attendee__c", "defaultFieldValues": {
+}}</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>SDGAction2</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>{"entityApiName": "Contact", "defaultFieldValues": {
+"AccountId" : "#parentrecordId#"
+}}</t>
+  </si>
+  <si>
+    <t>Member__r.Name</t>
+  </si>
+  <si>
+    <t>Type__c</t>
   </si>
 </sst>
 </file>
@@ -2173,7 +2216,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2283,6 +2326,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2617,21 +2663,21 @@
         <v>14</v>
       </c>
       <c r="K1" s="13" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="L1" s="13" t="s">
         <v>344</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="B2" t="s">
         <v>639</v>
-      </c>
-      <c r="B2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2664,7 +2710,7 @@
         <v>321</v>
       </c>
       <c r="E5" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -2721,7 +2767,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B11" t="s">
         <v>382</v>
@@ -2776,7 +2822,7 @@
         <v>385</v>
       </c>
       <c r="H16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I16" t="s">
         <v>381</v>
@@ -2800,7 +2846,7 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B19" t="s">
         <v>385</v>
@@ -2808,65 +2854,65 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B20" t="s">
         <v>385</v>
       </c>
       <c r="H20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="B21" t="s">
         <v>455</v>
       </c>
-      <c r="B21" t="s">
+      <c r="H21" t="s">
         <v>456</v>
-      </c>
-      <c r="H21" t="s">
-        <v>457</v>
       </c>
       <c r="I21" t="s">
         <v>381</v>
       </c>
       <c r="J21" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K21" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B22" t="s">
+        <v>455</v>
+      </c>
+      <c r="K22" t="s">
         <v>456</v>
-      </c>
-      <c r="K22" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B23" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B25" t="s">
         <v>349</v>
@@ -2880,101 +2926,101 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B26" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F26" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="B27" t="s">
+        <v>455</v>
+      </c>
+      <c r="F27" t="s">
         <v>486</v>
-      </c>
-      <c r="B27" t="s">
-        <v>456</v>
-      </c>
-      <c r="F27" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B28" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B29" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
+        <v>489</v>
+      </c>
+      <c r="B30" t="s">
         <v>490</v>
       </c>
-      <c r="B30" t="s">
+      <c r="F30" t="s">
         <v>491</v>
-      </c>
-      <c r="F30" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="B32" t="s">
         <v>497</v>
-      </c>
-      <c r="B32" t="s">
-        <v>498</v>
       </c>
       <c r="E32">
         <v>-20</v>
       </c>
       <c r="L32" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="B33" t="s">
         <v>539</v>
-      </c>
-      <c r="B33" t="s">
-        <v>540</v>
       </c>
       <c r="E33">
         <v>-25</v>
       </c>
       <c r="L33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
+        <v>587</v>
+      </c>
+      <c r="B34" t="s">
         <v>588</v>
-      </c>
-      <c r="B34" t="s">
-        <v>589</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K34" t="s">
         <v>349</v>
@@ -2982,16 +3028,16 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="B35" t="s">
         <v>591</v>
-      </c>
-      <c r="B35" t="s">
-        <v>592</v>
       </c>
       <c r="E35">
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K35" t="s">
         <v>349</v>
@@ -2999,16 +3045,16 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="B36" t="s">
         <v>593</v>
-      </c>
-      <c r="B36" t="s">
-        <v>594</v>
       </c>
       <c r="E36">
         <v>2</v>
       </c>
       <c r="F36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K36" t="s">
         <v>349</v>
@@ -3016,59 +3062,59 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
+        <v>594</v>
+      </c>
+      <c r="B37" t="s">
         <v>595</v>
-      </c>
-      <c r="B37" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="J38" t="s">
         <v>597</v>
-      </c>
-      <c r="J38" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
+        <v>598</v>
+      </c>
+      <c r="B39" t="s">
         <v>599</v>
       </c>
-      <c r="B39" t="s">
-        <v>600</v>
-      </c>
       <c r="J39" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B40" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F40" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="J40" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="L41" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>531</v>
+      </c>
+      <c r="M42" t="s">
         <v>532</v>
-      </c>
-      <c r="M42" t="s">
-        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -3125,7 +3171,7 @@
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -3187,7 +3233,7 @@
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -3199,10 +3245,10 @@
         <v>153</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>154</v>
@@ -3264,7 +3310,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -3279,7 +3325,7 @@
         <v>176</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>177</v>
@@ -3299,7 +3345,7 @@
         <v>181</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>182</v>
@@ -3319,7 +3365,7 @@
         <v>186</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>187</v>
@@ -3382,7 +3428,7 @@
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D3" s="32"/>
       <c r="E3" s="31"/>
@@ -3411,17 +3457,17 @@
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="49" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D6" s="32"/>
       <c r="E6" s="31"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>168</v>
@@ -3432,10 +3478,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="B8" t="s">
         <v>542</v>
-      </c>
-      <c r="B8" t="s">
-        <v>543</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>168</v>
@@ -3446,10 +3492,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>543</v>
+      </c>
+      <c r="B9" t="s">
         <v>544</v>
-      </c>
-      <c r="B9" t="s">
-        <v>545</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>168</v>
@@ -3460,10 +3506,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="B10" t="s">
         <v>546</v>
-      </c>
-      <c r="B10" t="s">
-        <v>547</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>168</v>
@@ -3474,10 +3520,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="B11" t="s">
         <v>548</v>
-      </c>
-      <c r="B11" t="s">
-        <v>549</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>168</v>
@@ -3488,10 +3534,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="B12" t="s">
         <v>550</v>
-      </c>
-      <c r="B12" t="s">
-        <v>551</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>168</v>
@@ -3502,10 +3548,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B13" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>168</v>
@@ -3516,10 +3562,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>168</v>
@@ -3530,10 +3576,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B15" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>168</v>
@@ -3544,10 +3590,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B16" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>168</v>
@@ -3558,10 +3604,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>168</v>
@@ -3572,10 +3618,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B18" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>168</v>
@@ -3586,10 +3632,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B19" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>168</v>
@@ -3600,10 +3646,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>168</v>
@@ -3614,10 +3660,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B21" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>168</v>
@@ -3628,10 +3674,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B22" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>168</v>
@@ -3642,10 +3688,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>168</v>
@@ -3656,10 +3702,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B24" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>168</v>
@@ -3670,10 +3716,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B25" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>168</v>
@@ -3684,10 +3730,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="B26" t="s">
         <v>622</v>
-      </c>
-      <c r="B26" t="s">
-        <v>623</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>168</v>
@@ -3698,10 +3744,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
+        <v>623</v>
+      </c>
+      <c r="B27" t="s">
         <v>624</v>
-      </c>
-      <c r="B27" t="s">
-        <v>625</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>168</v>
@@ -3714,7 +3760,7 @@
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -3726,16 +3772,16 @@
         <v>167</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>168</v>
       </c>
       <c r="D30" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -3780,7 +3826,7 @@
     <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -3810,26 +3856,26 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>517</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>518</v>
       </c>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>519</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>520</v>
       </c>
       <c r="C9" s="22"/>
     </row>
@@ -3944,7 +3990,7 @@
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
       <c r="D3" s="9" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -4002,7 +4048,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
       <c r="D7" s="9" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -4023,14 +4069,14 @@
     </row>
     <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
@@ -4042,16 +4088,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -4065,166 +4112,183 @@
         <v>141</v>
       </c>
       <c r="F1" s="32" t="s">
+        <v>660</v>
+      </c>
+      <c r="G1" s="32" t="s">
         <v>661</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>662</v>
       </c>
-      <c r="H1" s="32" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="19" t="s">
-        <v>139</v>
-      </c>
+    </row>
+    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>134</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C9" s="19" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C9" s="20" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="9" t="s">
-        <v>631</v>
-      </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="13"/>
-    </row>
-    <row r="15" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="B15" s="50" t="s">
-        <v>648</v>
-      </c>
-      <c r="C15" s="50" t="s">
-        <v>649</v>
-      </c>
-      <c r="G15" s="50" t="s">
-        <v>650</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>651</v>
-      </c>
+    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="9" t="s">
+        <v>630</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="13"/>
     </row>
     <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="G16" s="50" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="H16" s="50" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B17" s="50" t="s">
+        <v>652</v>
+      </c>
+      <c r="C17" s="50" t="s">
+        <v>653</v>
+      </c>
+      <c r="G17" s="50" t="s">
+        <v>654</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>652</v>
+      </c>
+      <c r="C18" s="50" t="s">
         <v>657</v>
       </c>
-      <c r="B17" s="50" t="s">
-        <v>653</v>
-      </c>
-      <c r="C17" s="50" t="s">
+      <c r="F18" s="50" t="s">
         <v>658</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="G18" s="50" t="s">
+        <v>649</v>
+      </c>
+      <c r="H18" s="50" t="s">
         <v>659</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>650</v>
-      </c>
-      <c r="H17" s="50" t="s">
-        <v>660</v>
       </c>
     </row>
   </sheetData>
@@ -4290,7 +4354,7 @@
         <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D2" t="s">
         <v>301</v>
@@ -4305,7 +4369,7 @@
         <v>302</v>
       </c>
       <c r="H2" s="29" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="I2" t="s">
         <v>33</v>
@@ -4334,7 +4398,7 @@
         <v>305</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I3" t="s">
         <v>323</v>
@@ -4363,7 +4427,7 @@
         <v>305</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I4" t="s">
         <v>324</v>
@@ -4379,7 +4443,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4422,7 +4486,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4475,7 +4539,7 @@
         <v>360</v>
       </c>
       <c r="B9" t="s">
-        <v>349</v>
+        <v>676</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -4483,7 +4547,7 @@
         <v>361</v>
       </c>
       <c r="B10" t="s">
-        <v>472</v>
+        <v>675</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -4499,10 +4563,10 @@
         <v>367</v>
       </c>
       <c r="B12" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="C12" s="27" t="s">
         <v>416</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -4547,7 +4611,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4561,7 +4625,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>96</v>
@@ -4583,7 +4647,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -4592,169 +4656,169 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B4" t="s">
         <v>419</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>420</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>421</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>422</v>
-      </c>
-      <c r="E4" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C5" t="s">
         <v>420</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>421</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>422</v>
-      </c>
-      <c r="E5" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B6" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" t="s">
         <v>420</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>421</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>422</v>
-      </c>
-      <c r="E6" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" t="s">
         <v>420</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>421</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>422</v>
-      </c>
-      <c r="E7" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B8" t="s">
+        <v>419</v>
+      </c>
+      <c r="C8" t="s">
         <v>420</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>421</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>422</v>
-      </c>
-      <c r="E8" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B9" t="s">
+        <v>419</v>
+      </c>
+      <c r="C9" t="s">
         <v>420</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>421</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>422</v>
-      </c>
-      <c r="E9" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B10" t="s">
+        <v>419</v>
+      </c>
+      <c r="C10" t="s">
         <v>420</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>421</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>422</v>
-      </c>
-      <c r="E10" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B11" t="s">
+        <v>419</v>
+      </c>
+      <c r="C11" t="s">
         <v>420</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>421</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>422</v>
-      </c>
-      <c r="E11" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B12" t="s">
+        <v>419</v>
+      </c>
+      <c r="C12" t="s">
         <v>420</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>421</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>422</v>
-      </c>
-      <c r="E12" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>625</v>
+      </c>
+      <c r="B13" t="s">
         <v>626</v>
       </c>
-      <c r="B13" t="s">
-        <v>627</v>
-      </c>
       <c r="C13" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D13" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -4781,16 +4845,16 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>430</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>431</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>368</v>
@@ -4799,7 +4863,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="9"/>
@@ -4808,222 +4872,222 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C3" t="s">
         <v>414</v>
       </c>
       <c r="D3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F3" t="s">
         <v>433</v>
-      </c>
-      <c r="F3" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C4" t="s">
         <v>414</v>
       </c>
       <c r="D4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C5" t="s">
         <v>414</v>
       </c>
       <c r="D5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F5" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C6" t="s">
         <v>414</v>
       </c>
       <c r="D6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E6" t="s">
+        <v>432</v>
+      </c>
+      <c r="F6" t="s">
         <v>433</v>
-      </c>
-      <c r="F6" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C7" t="s">
         <v>414</v>
       </c>
       <c r="D7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B8" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C8" t="s">
         <v>414</v>
       </c>
       <c r="D8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C9" t="s">
         <v>414</v>
       </c>
       <c r="D9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E9" t="s">
+        <v>432</v>
+      </c>
+      <c r="F9" t="s">
         <v>433</v>
-      </c>
-      <c r="F9" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C10" t="s">
         <v>414</v>
       </c>
       <c r="D10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C11" t="s">
         <v>414</v>
       </c>
       <c r="D11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E11" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F11" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B12" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C12" t="s">
         <v>414</v>
       </c>
       <c r="D12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E12" t="s">
+        <v>432</v>
+      </c>
+      <c r="F12" t="s">
         <v>433</v>
-      </c>
-      <c r="F12" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C13" t="s">
         <v>414</v>
       </c>
       <c r="D13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F13" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -5149,7 +5213,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
@@ -5163,7 +5227,7 @@
     <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C3" s="13"/>
       <c r="D3" s="9"/>
@@ -5172,112 +5236,193 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B4" t="s">
         <v>501</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>502</v>
-      </c>
-      <c r="C4" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>503</v>
+      </c>
+      <c r="B5" t="s">
         <v>504</v>
       </c>
-      <c r="B5" t="s">
-        <v>505</v>
-      </c>
       <c r="C5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>505</v>
+      </c>
+      <c r="B6" t="s">
         <v>506</v>
       </c>
-      <c r="B6" t="s">
-        <v>507</v>
-      </c>
       <c r="C6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>507</v>
+      </c>
+      <c r="B7" t="s">
         <v>508</v>
       </c>
-      <c r="B7" t="s">
-        <v>509</v>
-      </c>
       <c r="C7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B8" t="s">
         <v>399</v>
       </c>
       <c r="C8" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B9" t="s">
         <v>511</v>
       </c>
-      <c r="B9" t="s">
-        <v>512</v>
-      </c>
       <c r="C9" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>631</v>
+      </c>
+      <c r="B10" t="s">
         <v>632</v>
       </c>
-      <c r="B10" t="s">
-        <v>633</v>
-      </c>
       <c r="C10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B11" t="s">
         <v>398</v>
       </c>
       <c r="C11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>634</v>
+      </c>
+      <c r="B12" t="s">
         <v>635</v>
       </c>
-      <c r="B12" t="s">
-        <v>636</v>
-      </c>
       <c r="C12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>636</v>
+      </c>
+      <c r="B13" t="s">
         <v>637</v>
       </c>
-      <c r="B13" t="s">
-        <v>638</v>
-      </c>
       <c r="C13" t="s">
-        <v>619</v>
+        <v>618</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>667</v>
+      </c>
+      <c r="B2" t="s">
+        <v>668</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>669</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>670</v>
+      </c>
+      <c r="F2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B3" t="s">
+        <v>673</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E3" s="56" t="s">
+        <v>674</v>
+      </c>
+      <c r="F3" t="s">
+        <v>671</v>
       </c>
     </row>
   </sheetData>
@@ -5862,7 +6007,7 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -5870,7 +6015,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
@@ -5879,13 +6024,13 @@
         <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>41</v>
       </c>
       <c r="G35" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -7930,7 +8075,7 @@
     <row r="3" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -8939,7 +9084,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -8950,7 +9095,7 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C5" t="s">
         <v>33</v>
@@ -8961,7 +9106,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -8970,7 +9115,7 @@
     <row r="8" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -9132,17 +9277,17 @@
     <row r="24" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>602</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>603</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>79</v>
@@ -9150,10 +9295,10 @@
     </row>
     <row r="26" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>604</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>605</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>79</v>
@@ -9177,14 +9322,14 @@
     <row r="30" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B31" t="s">
         <v>395</v>
@@ -9195,10 +9340,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B32" t="s">
         <v>449</v>
-      </c>
-      <c r="B32" t="s">
-        <v>450</v>
       </c>
       <c r="C32" t="s">
         <v>292</v>
@@ -9207,7 +9352,7 @@
     <row r="34" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -9217,7 +9362,7 @@
         <v>146</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C35" s="22" t="s">
         <v>33</v>
@@ -9225,10 +9370,10 @@
     </row>
     <row r="36" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
+        <v>514</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>515</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>516</v>
       </c>
       <c r="C36" s="22"/>
     </row>
@@ -9308,10 +9453,10 @@
         <v>346</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -11322,7 +11467,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -12336,10 +12481,10 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -12355,7 +12500,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="7"/>
@@ -12505,7 +12650,7 @@
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="7"/>
@@ -12517,19 +12662,19 @@
     </row>
     <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
+        <v>605</v>
+      </c>
+      <c r="B18" s="50" t="s">
         <v>606</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="C18" s="50" t="s">
         <v>607</v>
       </c>
-      <c r="C18" s="50" t="s">
+      <c r="D18" s="50" t="s">
+        <v>602</v>
+      </c>
+      <c r="E18" s="54" t="s">
         <v>608</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>603</v>
-      </c>
-      <c r="E18" s="54" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -12539,7 +12684,7 @@
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="7"/>
@@ -12554,7 +12699,7 @@
         <v>394</v>
       </c>
       <c r="B21" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C21" t="s">
         <v>109</v>
@@ -12583,7 +12728,7 @@
         <v>400</v>
       </c>
       <c r="B22" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C22" t="s">
         <v>112</v>
@@ -12612,7 +12757,7 @@
         <v>403</v>
       </c>
       <c r="B23" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C23" t="s">
         <v>116</v>
@@ -12641,7 +12786,7 @@
         <v>405</v>
       </c>
       <c r="B24" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C24" t="s">
         <v>119</v>
@@ -12670,7 +12815,7 @@
         <v>407</v>
       </c>
       <c r="B25" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C25" t="s">
         <v>408</v>
@@ -12696,7 +12841,7 @@
         <v>409</v>
       </c>
       <c r="B26" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C26" t="s">
         <v>410</v>
@@ -12722,7 +12867,7 @@
         <v>411</v>
       </c>
       <c r="B27" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C27" t="s">
         <v>412</v>
@@ -12745,13 +12890,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>535</v>
+      </c>
+      <c r="B28" t="s">
         <v>536</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>537</v>
-      </c>
-      <c r="C28" t="s">
-        <v>538</v>
       </c>
       <c r="D28" t="s">
         <v>395</v>
@@ -12803,7 +12948,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>14</v>
@@ -12818,7 +12963,7 @@
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="7"/>
@@ -12830,10 +12975,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -12913,7 +13058,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="3"/>
@@ -12927,10 +13072,10 @@
         <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D4" t="s">
         <v>60</v>
@@ -12944,10 +13089,10 @@
         <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D5" t="s">
         <v>60</v>
@@ -12966,7 +13111,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
@@ -12977,10 +13122,10 @@
     </row>
     <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
+        <v>609</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>610</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>611</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>60</v>
@@ -12994,7 +13139,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="3"/>
@@ -13008,7 +13153,7 @@
         <v>147</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>60</v>
@@ -13022,7 +13167,7 @@
         <v>148</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>60</v>
@@ -15128,7 +15273,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -16159,7 +16304,7 @@
         <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -16171,7 +16316,7 @@
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:1026" x14ac:dyDescent="0.25">
@@ -16206,7 +16351,7 @@
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -16320,7 +16465,7 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -16345,7 +16490,7 @@
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -16357,7 +16502,7 @@
         <v>149</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>30</v>
@@ -16409,7 +16554,7 @@
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -16424,7 +16569,7 @@
         <v>159</v>
       </c>
       <c r="C4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>160</v>
@@ -16441,13 +16586,13 @@
         <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>163</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel for Module 3 & Module 7
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="942">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="976">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -1889,21 +1889,12 @@
     <t>M3MEETING1</t>
   </si>
   <si>
-    <t>Reliance</t>
-  </si>
-  <si>
     <t>Reliance Group</t>
   </si>
   <si>
-    <t>Ambani</t>
-  </si>
-  <si>
     <t>M3CON2</t>
   </si>
   <si>
-    <t>Kumar</t>
-  </si>
-  <si>
     <t>M3INS3</t>
   </si>
   <si>
@@ -1922,33 +1913,12 @@
     <t>M3INS8</t>
   </si>
   <si>
-    <t>Walmart</t>
-  </si>
-  <si>
-    <t>Company 1</t>
-  </si>
-  <si>
-    <t>Fund Manager 1</t>
-  </si>
-  <si>
-    <t>Indi Investor</t>
-  </si>
-  <si>
-    <t>Lender 1</t>
-  </si>
-  <si>
     <t>Fund Manager</t>
   </si>
   <si>
-    <t>Fund Manager's Fund</t>
-  </si>
-  <si>
     <t>Individual Investor</t>
   </si>
   <si>
-    <t>Fund Managers Fund 1</t>
-  </si>
-  <si>
     <t>Parent_Institution</t>
   </si>
   <si>
@@ -2177,9 +2147,6 @@
     <t>Test Deal 6</t>
   </si>
   <si>
-    <t>Due Dilligence</t>
-  </si>
-  <si>
     <t>M6Deal7</t>
   </si>
   <si>
@@ -2354,9 +2321,6 @@
     <t>60&lt;break&gt;-10&lt;break&gt;42&lt;break&gt;-10&lt;break&gt;</t>
   </si>
   <si>
-    <t>Test1Fund&lt;break&gt;Test1Fund of Funds</t>
-  </si>
-  <si>
     <t>M3Tc026_1_DeActivateARecordTypeForInstitution_Action</t>
   </si>
   <si>
@@ -2387,9 +2351,6 @@
     <t>Test Deal New</t>
   </si>
   <si>
-    <t>Test1Custom Object 1&lt;break&gt;Test1Custom Object 2</t>
-  </si>
-  <si>
     <t>M3Tc029_VerifyWhereChildNodeIsMovedFromOneParentToAnotherInNavigationMenu</t>
   </si>
   <si>
@@ -2399,18 +2360,9 @@
     <t>Parent_Account1&lt;break&gt;Parent_Account2</t>
   </si>
   <si>
-    <t>Aman Institute</t>
-  </si>
-  <si>
     <t>M3CON3</t>
   </si>
   <si>
-    <t>Ton</t>
-  </si>
-  <si>
-    <t>Reliance Digital</t>
-  </si>
-  <si>
     <t>M3PS1</t>
   </si>
   <si>
@@ -2418,9 +2370,6 @@
   </si>
   <si>
     <t>M3CON4</t>
-  </si>
-  <si>
-    <t>Nade</t>
   </si>
   <si>
     <t>M3INS9</t>
@@ -2834,36 +2783,6 @@
     <t>M3Tc034_1_VerifyTheFunctionalityByrenamingAndDeletingandRemovingUtilityItemCustomLabelintheCustomnavigationMenu</t>
   </si>
   <si>
-    <t>AATestAman</t>
-  </si>
-  <si>
-    <t>navatariptesting+15638@gmail.com</t>
-  </si>
-  <si>
-    <t>TestMukesh</t>
-  </si>
-  <si>
-    <t>navatariptesting+8709@gmail.com</t>
-  </si>
-  <si>
-    <t>TestDon</t>
-  </si>
-  <si>
-    <t>TestSatty</t>
-  </si>
-  <si>
-    <t>TestCst Record1</t>
-  </si>
-  <si>
-    <t>TestRelianced Fund</t>
-  </si>
-  <si>
-    <t>TestRelaince Fundraising</t>
-  </si>
-  <si>
-    <t>TestReliance Partner</t>
-  </si>
-  <si>
     <t>TestCall</t>
   </si>
   <si>
@@ -2892,6 +2811,189 @@
   </si>
   <si>
     <t>TestNew Interactions- Task</t>
+  </si>
+  <si>
+    <t>M6LSCFUNDR2</t>
+  </si>
+  <si>
+    <t>Test locale</t>
+  </si>
+  <si>
+    <t>Follow up Diligence</t>
+  </si>
+  <si>
+    <t>M6LSCFUNDR3</t>
+  </si>
+  <si>
+    <t>Test locale 1</t>
+  </si>
+  <si>
+    <t>M6LSCFUNDR4</t>
+  </si>
+  <si>
+    <t>Test locale 2</t>
+  </si>
+  <si>
+    <t>M6LSCFUNDR5</t>
+  </si>
+  <si>
+    <t>Test locale 3</t>
+  </si>
+  <si>
+    <t>Fund Manager’s Fund</t>
+  </si>
+  <si>
+    <t>Due Diligence</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>ATest1Fund&lt;break&gt;ATest1Fund of Funds</t>
+  </si>
+  <si>
+    <t>ATest1Custom Object 1&lt;break&gt;ATest1Custom Object 2</t>
+  </si>
+  <si>
+    <t>AAATestAman Institute</t>
+  </si>
+  <si>
+    <t>AAATestReliance Group</t>
+  </si>
+  <si>
+    <t>AAATestWalmart</t>
+  </si>
+  <si>
+    <t>AAATestCompany 1</t>
+  </si>
+  <si>
+    <t>AAATestFund Manager 1</t>
+  </si>
+  <si>
+    <t>AAATestFund Managers Fund 1</t>
+  </si>
+  <si>
+    <t>AAATestIndi Investor</t>
+  </si>
+  <si>
+    <t>AAATestLender 1</t>
+  </si>
+  <si>
+    <t>AAATestReliance Digital</t>
+  </si>
+  <si>
+    <t>AAATestReliance</t>
+  </si>
+  <si>
+    <t>AAATestAman</t>
+  </si>
+  <si>
+    <t>AAATestKumar</t>
+  </si>
+  <si>
+    <t>navatariptesting+95419@gmail.com</t>
+  </si>
+  <si>
+    <t>AAATestMukesh</t>
+  </si>
+  <si>
+    <t>AAATestAmbani</t>
+  </si>
+  <si>
+    <t>navatariptesting+30150@gmail.com</t>
+  </si>
+  <si>
+    <t>AAATestDon</t>
+  </si>
+  <si>
+    <t>AAATestTon</t>
+  </si>
+  <si>
+    <t>AAATestSatty</t>
+  </si>
+  <si>
+    <t>AAATestNade</t>
+  </si>
+  <si>
+    <t>AAATestCst Record1</t>
+  </si>
+  <si>
+    <t>AAATestRelianced Fund</t>
+  </si>
+  <si>
+    <t>M3DEAL1</t>
+  </si>
+  <si>
+    <t>AAATestJio Deal</t>
+  </si>
+  <si>
+    <t>AAATestRelaince Fundraising</t>
+  </si>
+  <si>
+    <t>AAATestReliance Partner</t>
+  </si>
+  <si>
+    <t>Module7</t>
+  </si>
+  <si>
+    <t>M7INS1</t>
+  </si>
+  <si>
+    <t>AAM7TestAlpha Tech</t>
+  </si>
+  <si>
+    <t>M7CON1</t>
+  </si>
+  <si>
+    <t>AAM7TestChriss</t>
+  </si>
+  <si>
+    <t>Vokes</t>
+  </si>
+  <si>
+    <t>navatariptesting+11679@gmail.com</t>
+  </si>
+  <si>
+    <t>M7CON2</t>
+  </si>
+  <si>
+    <t>AAM7TestTom</t>
+  </si>
+  <si>
+    <t>Latham</t>
+  </si>
+  <si>
+    <t>navatariptesting+18785@gmail.com</t>
+  </si>
+  <si>
+    <t>M7CON3</t>
+  </si>
+  <si>
+    <t>AAM7TestJames</t>
+  </si>
+  <si>
+    <t>Rose</t>
+  </si>
+  <si>
+    <t>navatariptesting+49153@gmail.com</t>
+  </si>
+  <si>
+    <t>M7Task1</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Task-1</t>
+  </si>
+  <si>
+    <t>9/1/2021</t>
+  </si>
+  <si>
+    <t>M7Task2</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Task-2</t>
+  </si>
+  <si>
+    <t>9/4/2021</t>
   </si>
 </sst>
 </file>
@@ -3454,7 +3556,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD17"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3548,29 +3650,29 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>643</v>
+        <v>633</v>
       </c>
       <c r="B6" t="s">
-        <v>760</v>
+        <v>749</v>
       </c>
       <c r="D6" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>644</v>
+        <v>634</v>
       </c>
       <c r="B7" t="s">
-        <v>762</v>
+        <v>751</v>
       </c>
       <c r="E7" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="B8" t="s">
         <v>308</v>
@@ -3578,7 +3680,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>646</v>
+        <v>636</v>
       </c>
       <c r="B9" t="s">
         <v>57</v>
@@ -3590,7 +3692,7 @@
         <v>343</v>
       </c>
       <c r="J9" t="s">
-        <v>764</v>
+        <v>927</v>
       </c>
       <c r="K9" t="s">
         <v>402</v>
@@ -3598,7 +3700,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
@@ -3609,15 +3711,15 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>648</v>
+        <v>638</v>
       </c>
       <c r="J11" t="s">
-        <v>775</v>
+        <v>928</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>765</v>
+        <v>753</v>
       </c>
       <c r="J12" t="s">
         <v>285</v>
@@ -3625,15 +3727,15 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>766</v>
+        <v>754</v>
       </c>
       <c r="B13" t="s">
-        <v>767</v>
+        <v>755</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>768</v>
+        <v>756</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -3641,13 +3743,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>776</v>
+        <v>763</v>
       </c>
       <c r="B15" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
       <c r="F15" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
       <c r="K15" t="s">
         <v>401</v>
@@ -3655,10 +3757,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>769</v>
+        <v>757</v>
       </c>
       <c r="B16" t="s">
-        <v>770</v>
+        <v>758</v>
       </c>
       <c r="K16" t="s">
         <v>401</v>
@@ -3666,13 +3768,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>921</v>
+        <v>904</v>
       </c>
       <c r="B17" t="s">
-        <v>770</v>
+        <v>758</v>
       </c>
       <c r="D17" t="s">
-        <v>771</v>
+        <v>759</v>
       </c>
     </row>
   </sheetData>
@@ -3777,13 +3879,14 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
@@ -3851,7 +3954,7 @@
         <v>314</v>
       </c>
       <c r="D6" s="59" t="s">
-        <v>733</v>
+        <v>722</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>319</v>
@@ -3868,10 +3971,10 @@
         <v>339</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>319</v>
+        <v>775</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -3901,47 +4004,47 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>790</v>
+        <v>773</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>793</v>
+        <v>776</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>734</v>
+        <v>723</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>822</v>
+        <v>805</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>823</v>
+        <v>806</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>823</v>
+        <v>806</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>151</v>
@@ -3949,13 +4052,13 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>824</v>
+        <v>807</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>825</v>
+        <v>808</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>825</v>
+        <v>808</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>151</v>
@@ -4032,13 +4135,13 @@
         <v>573</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>828</v>
+        <v>811</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>795</v>
+        <v>778</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>796</v>
+        <v>779</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>173</v>
@@ -4052,7 +4155,7 @@
         <v>175</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>830</v>
+        <v>813</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>176</v>
@@ -4072,10 +4175,10 @@
         <v>180</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>831</v>
+        <v>814</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>797</v>
+        <v>780</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>181</v>
@@ -4483,16 +4586,16 @@
         <v>164</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>831</v>
+        <v>814</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>833</v>
+        <v>816</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>828</v>
+        <v>811</v>
       </c>
     </row>
   </sheetData>
@@ -4503,10 +4606,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4567,45 +4670,55 @@
     <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
     <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>444</v>
+        <v>767</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>445</v>
+        <v>954</v>
       </c>
       <c r="C8" s="22"/>
     </row>
     <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>446</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>447</v>
-      </c>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="22"/>
     </row>
     <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
     <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>783</v>
+        <v>444</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>931</v>
+        <v>445</v>
       </c>
       <c r="C12" s="22"/>
+    </row>
+    <row r="13" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>447</v>
+      </c>
+      <c r="C13" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4824,7 +4937,7 @@
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,7 +5091,7 @@
         <v>535</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>932</v>
+        <v>905</v>
       </c>
       <c r="G16" s="50" t="s">
         <v>537</v>
@@ -4995,7 +5108,7 @@
         <v>540</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>933</v>
+        <v>906</v>
       </c>
       <c r="G17" s="50" t="s">
         <v>541</v>
@@ -5012,7 +5125,7 @@
         <v>540</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>934</v>
+        <v>907</v>
       </c>
       <c r="F18" s="50" t="s">
         <v>544</v>
@@ -5105,7 +5218,7 @@
         <v>561</v>
       </c>
       <c r="I2" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -5131,7 +5244,7 @@
         <v>295</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>631</v>
+        <v>621</v>
       </c>
       <c r="I3" t="s">
         <v>35</v>
@@ -5160,10 +5273,10 @@
         <v>295</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>632</v>
+        <v>622</v>
       </c>
       <c r="I4" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>
@@ -5272,7 +5385,7 @@
         <v>329</v>
       </c>
       <c r="B9" t="s">
-        <v>735</v>
+        <v>724</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5280,7 +5393,7 @@
         <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>736</v>
+        <v>725</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5307,7 +5420,7 @@
         <v>331</v>
       </c>
       <c r="B13" t="s">
-        <v>737</v>
+        <v>726</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5315,7 +5428,7 @@
         <v>332</v>
       </c>
       <c r="B14" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5323,7 +5436,7 @@
         <v>333</v>
       </c>
       <c r="B15" t="s">
-        <v>739</v>
+        <v>728</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5331,7 +5444,7 @@
         <v>334</v>
       </c>
       <c r="B16" t="s">
-        <v>740</v>
+        <v>729</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5347,50 +5460,50 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>798</v>
+        <v>781</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>799</v>
+        <v>782</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>800</v>
+        <v>783</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>801</v>
+        <v>784</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>802</v>
+        <v>785</v>
       </c>
       <c r="B21" s="61" t="s">
-        <v>803</v>
+        <v>786</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>804</v>
+        <v>787</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>737</v>
+        <v>726</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>805</v>
+        <v>788</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>738</v>
+        <v>727</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>806</v>
+        <v>789</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>807</v>
+        <v>790</v>
       </c>
     </row>
   </sheetData>
@@ -5712,36 +5825,36 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>637</v>
+        <v>627</v>
       </c>
       <c r="B5" t="s">
         <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>633</v>
+        <v>623</v>
       </c>
       <c r="D5" t="s">
-        <v>638</v>
+        <v>628</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>639</v>
+        <v>629</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
       <c r="B6" t="s">
         <v>573</v>
       </c>
       <c r="C6" t="s">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="D6" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -6303,10 +6416,10 @@
         <v>584</v>
       </c>
       <c r="B2" t="s">
-        <v>935</v>
+        <v>908</v>
       </c>
       <c r="C2" t="s">
-        <v>936</v>
+        <v>909</v>
       </c>
       <c r="D2" t="s">
         <v>585</v>
@@ -6379,10 +6492,10 @@
         <v>594</v>
       </c>
       <c r="B2" t="s">
-        <v>937</v>
+        <v>910</v>
       </c>
       <c r="C2" t="s">
-        <v>938</v>
+        <v>911</v>
       </c>
       <c r="D2" t="s">
         <v>595</v>
@@ -6411,10 +6524,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMJ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6450,10 +6563,10 @@
         <v>600</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>845</v>
+        <v>828</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>846</v>
+        <v>829</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>547</v>
@@ -7486,18 +7599,18 @@
       <c r="AMJ1" s="5"/>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="30" t="s">
         <v>606</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>604</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>939</v>
+        <v>912</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" t="s">
-        <v>772</v>
+        <v>760</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
@@ -8529,7 +8642,7 @@
         <v>604</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>940</v>
+        <v>913</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -9565,7 +9678,7 @@
         <v>604</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>941</v>
+        <v>914</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -10592,8 +10705,8 @@
       <c r="AMJ4" s="5"/>
     </row>
     <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>847</v>
+      <c r="A5" s="30" t="s">
+        <v>830</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>604</v>
@@ -10602,138 +10715,138 @@
         <v>536</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>848</v>
+        <v>831</v>
       </c>
       <c r="E5" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>850</v>
+        <v>833</v>
       </c>
       <c r="G5" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="19"/>
     </row>
     <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>852</v>
+        <v>835</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>853</v>
+        <v>836</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>854</v>
+        <v>837</v>
       </c>
       <c r="E6" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>855</v>
+        <v>838</v>
       </c>
       <c r="G6" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="19"/>
     </row>
     <row r="7" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>856</v>
+        <v>839</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>858</v>
+        <v>841</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>859</v>
+        <v>842</v>
       </c>
       <c r="E7" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>860</v>
+        <v>843</v>
       </c>
       <c r="G7" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>861</v>
+        <v>844</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>862</v>
+        <v>845</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="E8" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="G8" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>865</v>
+        <v>848</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>866</v>
+        <v>849</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>867</v>
+        <v>850</v>
       </c>
       <c r="E9" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>868</v>
+        <v>851</v>
       </c>
       <c r="G9" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>869</v>
+        <v>852</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>870</v>
+        <v>853</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="E10" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
@@ -10743,22 +10856,22 @@
     </row>
     <row r="11" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>873</v>
+        <v>856</v>
       </c>
       <c r="B11" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>874</v>
+        <v>857</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>875</v>
+        <v>858</v>
       </c>
       <c r="E11" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="G11" t="s">
         <v>369</v>
@@ -10768,22 +10881,22 @@
     </row>
     <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>877</v>
+        <v>860</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>878</v>
+        <v>861</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
       <c r="E12" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="G12" t="s">
         <v>369</v>
@@ -10793,22 +10906,22 @@
     </row>
     <row r="13" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>881</v>
+        <v>864</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>882</v>
+        <v>865</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="E13" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>884</v>
+        <v>867</v>
       </c>
       <c r="G13" t="s">
         <v>369</v>
@@ -10818,22 +10931,22 @@
     </row>
     <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>885</v>
+        <v>868</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>604</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>886</v>
+        <v>869</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>887</v>
+        <v>870</v>
       </c>
       <c r="E14" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="G14" t="s">
         <v>369</v>
@@ -10843,103 +10956,137 @@
     </row>
     <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>889</v>
+        <v>872</v>
       </c>
       <c r="B15" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>890</v>
+        <v>873</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>867</v>
+        <v>850</v>
       </c>
       <c r="E15" t="s">
-        <v>833</v>
+        <v>816</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="G15" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>891</v>
+        <v>874</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>857</v>
+        <v>840</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>892</v>
+        <v>875</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="E16" t="s">
-        <v>833</v>
+        <v>816</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="G16" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>893</v>
+        <v>876</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>894</v>
+        <v>877</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>859</v>
+        <v>842</v>
       </c>
       <c r="E17" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>860</v>
+        <v>843</v>
       </c>
       <c r="G17" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>896</v>
+        <v>879</v>
       </c>
       <c r="B18" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>897</v>
+        <v>880</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="E18" t="s">
-        <v>895</v>
+        <v>878</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="G18" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="30" t="s">
+        <v>970</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>971</v>
+      </c>
+      <c r="E20" t="s">
+        <v>972</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>973</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>974</v>
+      </c>
+      <c r="E21" t="s">
+        <v>975</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>605</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10973,22 +11120,22 @@
         <v>138</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>898</v>
+        <v>881</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>899</v>
+        <v>882</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>319</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>845</v>
+        <v>828</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>846</v>
+        <v>829</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>900</v>
+        <v>883</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -12003,262 +12150,262 @@
     </row>
     <row r="2" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>901</v>
+        <v>884</v>
       </c>
       <c r="B2" t="s">
         <v>536</v>
       </c>
       <c r="C2" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="D2" t="s">
-        <v>902</v>
+        <v>885</v>
       </c>
       <c r="E2" t="s">
-        <v>848</v>
+        <v>831</v>
       </c>
       <c r="F2" t="s">
-        <v>850</v>
+        <v>833</v>
       </c>
       <c r="G2" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H2" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
     </row>
     <row r="3" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>904</v>
+        <v>887</v>
       </c>
       <c r="B3" t="s">
         <v>321</v>
       </c>
       <c r="C3" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D3" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E3" t="s">
-        <v>854</v>
+        <v>837</v>
       </c>
       <c r="F3" t="s">
-        <v>855</v>
+        <v>838</v>
       </c>
       <c r="G3" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H3" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
     </row>
     <row r="4" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>906</v>
+        <v>889</v>
       </c>
       <c r="B4" t="s">
-        <v>907</v>
+        <v>890</v>
       </c>
       <c r="C4" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D4" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E4" t="s">
-        <v>859</v>
+        <v>842</v>
       </c>
       <c r="F4" t="s">
-        <v>860</v>
+        <v>843</v>
       </c>
       <c r="G4" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H4" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
     </row>
     <row r="5" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>908</v>
+        <v>891</v>
       </c>
       <c r="B5" t="s">
-        <v>909</v>
+        <v>892</v>
       </c>
       <c r="C5" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D5" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E5" t="s">
-        <v>863</v>
+        <v>846</v>
       </c>
       <c r="F5" t="s">
-        <v>864</v>
+        <v>847</v>
       </c>
       <c r="G5" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H5" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
     </row>
     <row r="6" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>910</v>
+        <v>893</v>
       </c>
       <c r="B6" t="s">
-        <v>862</v>
+        <v>845</v>
       </c>
       <c r="C6" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D6" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E6" t="s">
-        <v>867</v>
+        <v>850</v>
       </c>
       <c r="F6" t="s">
-        <v>868</v>
+        <v>851</v>
       </c>
       <c r="G6" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H6" t="s">
-        <v>903</v>
+        <v>886</v>
       </c>
     </row>
     <row r="7" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>911</v>
+        <v>894</v>
       </c>
       <c r="B7" t="s">
-        <v>866</v>
+        <v>849</v>
       </c>
       <c r="C7" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D7" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E7" t="s">
-        <v>871</v>
+        <v>854</v>
       </c>
       <c r="F7" t="s">
-        <v>872</v>
+        <v>855</v>
       </c>
       <c r="G7" t="s">
         <v>369</v>
       </c>
       <c r="H7" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
     </row>
     <row r="8" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>913</v>
+        <v>896</v>
       </c>
       <c r="B8" t="s">
-        <v>914</v>
+        <v>897</v>
       </c>
       <c r="C8" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D8" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E8" t="s">
-        <v>875</v>
+        <v>858</v>
       </c>
       <c r="F8" t="s">
-        <v>876</v>
+        <v>859</v>
       </c>
       <c r="G8" t="s">
         <v>369</v>
       </c>
       <c r="H8" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
     </row>
     <row r="9" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>915</v>
+        <v>898</v>
       </c>
       <c r="B9" t="s">
-        <v>916</v>
+        <v>899</v>
       </c>
       <c r="C9" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D9" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E9" t="s">
-        <v>879</v>
+        <v>862</v>
       </c>
       <c r="F9" t="s">
-        <v>880</v>
+        <v>863</v>
       </c>
       <c r="G9" t="s">
         <v>369</v>
       </c>
       <c r="H9" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
     </row>
     <row r="10" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>917</v>
+        <v>900</v>
       </c>
       <c r="B10" t="s">
-        <v>918</v>
+        <v>901</v>
       </c>
       <c r="C10" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D10" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E10" t="s">
-        <v>883</v>
+        <v>866</v>
       </c>
       <c r="F10" t="s">
-        <v>884</v>
+        <v>867</v>
       </c>
       <c r="G10" t="s">
         <v>369</v>
       </c>
       <c r="H10" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
     </row>
     <row r="11" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>919</v>
+        <v>902</v>
       </c>
       <c r="B11" t="s">
-        <v>920</v>
+        <v>903</v>
       </c>
       <c r="C11" t="s">
-        <v>849</v>
+        <v>832</v>
       </c>
       <c r="D11" t="s">
-        <v>905</v>
+        <v>888</v>
       </c>
       <c r="E11" t="s">
-        <v>887</v>
+        <v>870</v>
       </c>
       <c r="F11" t="s">
-        <v>888</v>
+        <v>871</v>
       </c>
       <c r="G11" t="s">
-        <v>851</v>
+        <v>834</v>
       </c>
       <c r="H11" t="s">
-        <v>912</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -12839,7 +12986,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="B33" t="s">
         <v>184</v>
@@ -12854,7 +13001,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>635</v>
+        <v>625</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -12869,7 +13016,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>636</v>
+        <v>626</v>
       </c>
       <c r="B35" t="s">
         <v>234</v>
@@ -12922,10 +13069,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO71"/>
+  <dimension ref="A1:ALO74"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12951,7 +13098,7 @@
         <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>629</v>
+        <v>619</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -16171,7 +16318,7 @@
         <v>504</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>779</v>
+        <v>929</v>
       </c>
       <c r="C25" t="s">
         <v>32</v>
@@ -16182,7 +16329,7 @@
         <v>505</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>610</v>
+        <v>930</v>
       </c>
       <c r="C26" t="s">
         <v>32</v>
@@ -16190,10 +16337,10 @@
     </row>
     <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>620</v>
+        <v>931</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
@@ -16201,10 +16348,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>621</v>
+        <v>932</v>
       </c>
       <c r="C28" t="s">
         <v>76</v>
@@ -16212,74 +16359,74 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>622</v>
+        <v>933</v>
       </c>
       <c r="C29" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>628</v>
+        <v>934</v>
       </c>
       <c r="C30" t="s">
-        <v>626</v>
+        <v>924</v>
       </c>
       <c r="E30" t="s">
-        <v>622</v>
+        <v>933</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>615</v>
+      </c>
+      <c r="B31" s="22" t="s">
+        <v>935</v>
+      </c>
+      <c r="C31" t="s">
         <v>618</v>
-      </c>
-      <c r="B31" s="22" t="s">
-        <v>623</v>
-      </c>
-      <c r="C31" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>624</v>
+        <v>936</v>
       </c>
       <c r="C32" t="s">
         <v>62</v>
       </c>
       <c r="E32" t="s">
-        <v>620</v>
+        <v>931</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>782</v>
+        <v>937</v>
       </c>
       <c r="C33" t="s">
         <v>62</v>
       </c>
       <c r="E33" s="22" t="s">
-        <v>779</v>
+        <v>929</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>609</v>
+        <v>938</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -16343,7 +16490,7 @@
         <v>143</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>828</v>
+        <v>811</v>
       </c>
       <c r="C43" s="22" t="s">
         <v>32</v>
@@ -16367,17 +16514,17 @@
     <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>651</v>
+        <v>641</v>
       </c>
       <c r="C48" s="22" t="s">
         <v>32</v>
@@ -16385,10 +16532,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>652</v>
+        <v>642</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
       <c r="C49" s="22" t="s">
         <v>76</v>
@@ -16397,10 +16544,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>654</v>
+        <v>644</v>
       </c>
       <c r="B50" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="C50" t="s">
         <v>76</v>
@@ -16408,10 +16555,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="B51" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="C51" t="s">
         <v>76</v>
@@ -16419,10 +16566,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="B52" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
       <c r="C52" t="s">
         <v>76</v>
@@ -16430,10 +16577,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="B53" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="C53" t="s">
         <v>76</v>
@@ -16441,10 +16588,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="B54" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="C54" t="s">
         <v>76</v>
@@ -16452,10 +16599,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="B55" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="C55" t="s">
         <v>76</v>
@@ -16463,10 +16610,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="B56" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
       <c r="C56" t="s">
         <v>76</v>
@@ -16474,10 +16621,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="B57" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="C57" t="s">
         <v>76</v>
@@ -16485,10 +16632,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="B58" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="C58" t="s">
         <v>76</v>
@@ -16496,10 +16643,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
       <c r="B59" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
       <c r="C59" t="s">
         <v>352</v>
@@ -16507,43 +16654,43 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="B60" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="C60" t="s">
-        <v>625</v>
+        <v>617</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="B61" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="C61" t="s">
-        <v>626</v>
+        <v>924</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="B62" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="C62" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="B63" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="C63" t="s">
         <v>285</v>
@@ -16551,78 +16698,97 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="B64" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="C64" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="B65" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="C65" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="B66" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="C66" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="B67" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="C67" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>810</v>
+        <v>793</v>
       </c>
       <c r="B68" t="s">
-        <v>808</v>
+        <v>791</v>
       </c>
       <c r="C68" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>811</v>
+        <v>794</v>
       </c>
       <c r="B69" t="s">
-        <v>809</v>
+        <v>792</v>
       </c>
       <c r="C69" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>817</v>
+        <v>800</v>
       </c>
       <c r="B71" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C71" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>956</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="C74" t="s">
         <v>32</v>
       </c>
     </row>
@@ -16633,10 +16799,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR40"/>
+  <dimension ref="A1:ALR46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD21"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16647,10 +16813,10 @@
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -19899,53 +20065,53 @@
         <v>506</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>922</v>
+        <v>939</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>613</v>
+        <v>940</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>779</v>
+        <v>929</v>
       </c>
       <c r="E18" t="s">
-        <v>923</v>
+        <v>941</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>924</v>
+        <v>942</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>611</v>
+        <v>943</v>
       </c>
       <c r="E19" t="s">
-        <v>925</v>
+        <v>944</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>926</v>
+        <v>945</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>781</v>
+        <v>946</v>
       </c>
       <c r="E20" s="54"/>
     </row>
     <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
-        <v>785</v>
+        <v>769</v>
       </c>
       <c r="B21" s="50" t="s">
-        <v>927</v>
+        <v>947</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>786</v>
+        <v>948</v>
       </c>
       <c r="E21" s="54"/>
     </row>
@@ -19989,7 +20155,7 @@
         <v>347</v>
       </c>
       <c r="I24" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J24" t="s">
         <v>349</v>
@@ -20018,7 +20184,7 @@
         <v>352</v>
       </c>
       <c r="I25" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J25" t="s">
         <v>349</v>
@@ -20047,7 +20213,7 @@
         <v>347</v>
       </c>
       <c r="I26" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J26" t="s">
         <v>349</v>
@@ -20076,7 +20242,7 @@
         <v>352</v>
       </c>
       <c r="I27" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J27" t="s">
         <v>349</v>
@@ -20102,7 +20268,7 @@
         <v>347</v>
       </c>
       <c r="I28" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J28" t="s">
         <v>349</v>
@@ -20128,7 +20294,7 @@
         <v>352</v>
       </c>
       <c r="I29" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J29" t="s">
         <v>349</v>
@@ -20154,7 +20320,7 @@
         <v>347</v>
       </c>
       <c r="I30" t="s">
-        <v>348</v>
+        <v>926</v>
       </c>
       <c r="J30" t="s">
         <v>349</v>
@@ -20193,19 +20359,19 @@
     </row>
     <row r="34" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
-        <v>826</v>
+        <v>809</v>
       </c>
       <c r="B34" s="50" t="s">
-        <v>829</v>
+        <v>812</v>
       </c>
       <c r="C34" s="50" t="s">
-        <v>827</v>
+        <v>810</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
       <c r="E34" t="s">
-        <v>832</v>
+        <v>815</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
@@ -20224,7 +20390,7 @@
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
-        <v>741</v>
+        <v>955</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="7"/>
@@ -20234,59 +20400,135 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>742</v>
-      </c>
-      <c r="B38" t="s">
-        <v>743</v>
-      </c>
-      <c r="C38" t="s">
-        <v>744</v>
-      </c>
-      <c r="E38" s="60" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>746</v>
-      </c>
-      <c r="B39" t="s">
-        <v>747</v>
-      </c>
-      <c r="C39" t="s">
-        <v>748</v>
-      </c>
-      <c r="E39" s="60" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>834</v>
-      </c>
-      <c r="B40" t="s">
-        <v>835</v>
-      </c>
-      <c r="E40" s="60"/>
-      <c r="K40" t="s">
+    <row r="38" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
+        <v>958</v>
+      </c>
+      <c r="B38" s="50" t="s">
+        <v>959</v>
+      </c>
+      <c r="C38" s="50" t="s">
+        <v>960</v>
+      </c>
+      <c r="D38" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="50" t="s">
+        <v>962</v>
+      </c>
+      <c r="B39" s="50" t="s">
+        <v>963</v>
+      </c>
+      <c r="C39" s="50" t="s">
+        <v>964</v>
+      </c>
+      <c r="D39" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E39" s="22" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="50" t="s">
+        <v>966</v>
+      </c>
+      <c r="B40" s="50" t="s">
+        <v>967</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>968</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>731</v>
+      </c>
+      <c r="B44" t="s">
+        <v>732</v>
+      </c>
+      <c r="C44" t="s">
+        <v>733</v>
+      </c>
+      <c r="E44" s="60" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>735</v>
+      </c>
+      <c r="B45" t="s">
+        <v>736</v>
+      </c>
+      <c r="C45" t="s">
+        <v>737</v>
+      </c>
+      <c r="E45" s="60" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>817</v>
+      </c>
+      <c r="B46" t="s">
+        <v>818</v>
+      </c>
+      <c r="E46" s="60"/>
+      <c r="K46" t="s">
         <v>555</v>
       </c>
-      <c r="L40" t="s">
-        <v>836</v>
-      </c>
-      <c r="M40" t="s">
-        <v>837</v>
-      </c>
-      <c r="N40" t="s">
-        <v>838</v>
+      <c r="L46" t="s">
+        <v>819</v>
+      </c>
+      <c r="M46" t="s">
+        <v>820</v>
+      </c>
+      <c r="N46" t="s">
+        <v>821</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E38" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
-    <hyperlink ref="E39" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E44" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E45" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E40" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20342,7 +20584,7 @@
         <v>508</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>928</v>
+        <v>949</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -20483,7 +20725,7 @@
         <v>507</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>929</v>
+        <v>950</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>57</v>
@@ -20539,7 +20781,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>649</v>
+        <v>639</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
@@ -20550,10 +20792,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>818</v>
+        <v>801</v>
       </c>
       <c r="B17" t="s">
-        <v>819</v>
+        <v>802</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>57</v>
@@ -20569,10 +20811,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML49"/>
+  <dimension ref="A1:AML55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:XFD49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23878,440 +24120,478 @@
       </c>
     </row>
     <row r="15" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4" t="s">
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>951</v>
+      </c>
+      <c r="B18" t="s">
+        <v>952</v>
+      </c>
+      <c r="C18" t="s">
+        <v>929</v>
+      </c>
+      <c r="D18" t="s">
+        <v>925</v>
+      </c>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:1026" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>363</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>364</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C22" t="s">
         <v>345</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4" t="s">
+    <row r="24" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>830</v>
-      </c>
-      <c r="D19" s="50" t="s">
+      <c r="B25" s="20" t="s">
+        <v>813</v>
+      </c>
+      <c r="D25" s="50" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4" t="s">
-        <v>691</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>692</v>
-      </c>
-      <c r="B23" t="s">
-        <v>693</v>
-      </c>
-      <c r="C23" t="s">
-        <v>651</v>
-      </c>
-      <c r="D23" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>694</v>
-      </c>
-      <c r="B24" t="s">
-        <v>695</v>
-      </c>
-      <c r="C24" t="s">
-        <v>653</v>
-      </c>
-      <c r="D24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>696</v>
-      </c>
-      <c r="B25" t="s">
-        <v>697</v>
-      </c>
-      <c r="C25" t="s">
-        <v>653</v>
-      </c>
-      <c r="D25" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>699</v>
-      </c>
-      <c r="B26" t="s">
-        <v>700</v>
-      </c>
-      <c r="C26" t="s">
-        <v>657</v>
-      </c>
-      <c r="D26" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>701</v>
-      </c>
-      <c r="B27" t="s">
-        <v>702</v>
-      </c>
-      <c r="C27" t="s">
-        <v>659</v>
-      </c>
-      <c r="D27" t="s">
-        <v>262</v>
-      </c>
-    </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>703</v>
-      </c>
-      <c r="B28" t="s">
-        <v>704</v>
-      </c>
-      <c r="C28" t="s">
-        <v>661</v>
-      </c>
-      <c r="D28" t="s">
-        <v>705</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>706</v>
+        <v>682</v>
       </c>
       <c r="B29" t="s">
-        <v>707</v>
+        <v>683</v>
       </c>
       <c r="C29" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="D29" t="s">
-        <v>708</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>709</v>
+        <v>684</v>
       </c>
       <c r="B30" t="s">
-        <v>710</v>
+        <v>685</v>
       </c>
       <c r="C30" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>711</v>
+        <v>686</v>
       </c>
       <c r="B31" t="s">
-        <v>712</v>
+        <v>687</v>
       </c>
       <c r="C31" t="s">
-        <v>667</v>
+        <v>643</v>
       </c>
       <c r="D31" t="s">
-        <v>262</v>
+        <v>688</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>713</v>
+        <v>689</v>
       </c>
       <c r="B32" t="s">
-        <v>714</v>
+        <v>690</v>
       </c>
       <c r="C32" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="D32" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>715</v>
+        <v>691</v>
       </c>
       <c r="B33" t="s">
-        <v>716</v>
+        <v>692</v>
       </c>
       <c r="C33" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="D33" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>717</v>
+        <v>693</v>
       </c>
       <c r="B34" t="s">
-        <v>718</v>
+        <v>694</v>
       </c>
       <c r="C34" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
       <c r="D34" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>719</v>
+        <v>695</v>
       </c>
       <c r="B35" t="s">
-        <v>720</v>
+        <v>696</v>
       </c>
       <c r="C35" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="D35" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>721</v>
+        <v>698</v>
       </c>
       <c r="B36" t="s">
-        <v>722</v>
+        <v>699</v>
       </c>
       <c r="C36" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
       <c r="D36" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>723</v>
+        <v>700</v>
       </c>
       <c r="B37" t="s">
-        <v>724</v>
+        <v>701</v>
       </c>
       <c r="C37" t="s">
-        <v>679</v>
+        <v>657</v>
       </c>
       <c r="D37" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>725</v>
+        <v>702</v>
       </c>
       <c r="B38" t="s">
-        <v>726</v>
+        <v>703</v>
       </c>
       <c r="C38" t="s">
-        <v>681</v>
+        <v>659</v>
       </c>
       <c r="D38" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>727</v>
+        <v>704</v>
       </c>
       <c r="B39" t="s">
-        <v>728</v>
+        <v>705</v>
       </c>
       <c r="C39" t="s">
-        <v>683</v>
+        <v>661</v>
       </c>
       <c r="D39" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>729</v>
+        <v>706</v>
       </c>
       <c r="B40" t="s">
-        <v>730</v>
+        <v>707</v>
       </c>
       <c r="C40" t="s">
-        <v>685</v>
+        <v>663</v>
       </c>
       <c r="D40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>731</v>
+        <v>708</v>
       </c>
       <c r="B41" t="s">
-        <v>732</v>
+        <v>709</v>
       </c>
       <c r="C41" t="s">
-        <v>690</v>
+        <v>665</v>
       </c>
       <c r="D41" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>773</v>
+        <v>710</v>
       </c>
       <c r="B42" t="s">
-        <v>774</v>
+        <v>711</v>
       </c>
       <c r="C42" t="s">
-        <v>688</v>
+        <v>667</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>812</v>
+        <v>712</v>
       </c>
       <c r="B43" t="s">
-        <v>814</v>
+        <v>713</v>
       </c>
       <c r="C43" t="s">
-        <v>808</v>
+        <v>669</v>
       </c>
       <c r="D43" t="s">
         <v>262</v>
       </c>
-      <c r="G43" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>813</v>
+        <v>714</v>
       </c>
       <c r="B44" t="s">
-        <v>815</v>
+        <v>715</v>
       </c>
       <c r="C44" t="s">
-        <v>809</v>
+        <v>671</v>
       </c>
       <c r="D44" t="s">
         <v>262</v>
       </c>
-      <c r="G44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4" t="s">
-        <v>750</v>
-      </c>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>716</v>
+      </c>
+      <c r="B45" t="s">
+        <v>717</v>
+      </c>
+      <c r="C45" t="s">
+        <v>673</v>
+      </c>
+      <c r="D45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>718</v>
+      </c>
+      <c r="B46" t="s">
+        <v>719</v>
+      </c>
+      <c r="C46" t="s">
+        <v>675</v>
+      </c>
+      <c r="D46" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>751</v>
+        <v>720</v>
       </c>
       <c r="B47" t="s">
-        <v>752</v>
+        <v>721</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>680</v>
       </c>
       <c r="D47" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>753</v>
+        <v>761</v>
       </c>
       <c r="B48" t="s">
-        <v>754</v>
+        <v>762</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>678</v>
       </c>
       <c r="D48" t="s">
-        <v>569</v>
+        <v>30</v>
+      </c>
+      <c r="F48" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>839</v>
+        <v>795</v>
       </c>
       <c r="B49" t="s">
-        <v>840</v>
-      </c>
-      <c r="I49" t="s">
+        <v>797</v>
+      </c>
+      <c r="C49" t="s">
+        <v>791</v>
+      </c>
+      <c r="D49" t="s">
+        <v>262</v>
+      </c>
+      <c r="G49" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>796</v>
+      </c>
+      <c r="B50" t="s">
+        <v>798</v>
+      </c>
+      <c r="C50" t="s">
+        <v>792</v>
+      </c>
+      <c r="D50" t="s">
+        <v>262</v>
+      </c>
+      <c r="G50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="3"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>740</v>
+      </c>
+      <c r="B53" t="s">
+        <v>741</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>742</v>
+      </c>
+      <c r="B54" t="s">
+        <v>743</v>
+      </c>
+      <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>822</v>
+      </c>
+      <c r="B55" t="s">
+        <v>823</v>
+      </c>
+      <c r="I55" t="s">
         <v>555</v>
       </c>
-      <c r="J49" t="s">
-        <v>836</v>
-      </c>
-      <c r="K49" t="s">
-        <v>837</v>
-      </c>
-      <c r="L49" t="s">
-        <v>841</v>
+      <c r="J55" t="s">
+        <v>819</v>
+      </c>
+      <c r="K55" t="s">
+        <v>820</v>
+      </c>
+      <c r="L55" t="s">
+        <v>824</v>
       </c>
     </row>
   </sheetData>
@@ -24323,7 +24603,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD7"/>
@@ -24335,9 +24615,9 @@
     <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -24345,7 +24625,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>755</v>
+        <v>744</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>12</v>
@@ -24368,38 +24648,38 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>756</v>
+        <v>745</v>
       </c>
       <c r="B2" t="s">
-        <v>757</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>758</v>
+        <v>747</v>
       </c>
       <c r="B3" t="s">
-        <v>759</v>
+        <v>748</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>842</v>
+        <v>825</v>
       </c>
       <c r="B4" t="s">
-        <v>843</v>
+        <v>826</v>
       </c>
       <c r="E4" t="s">
         <v>555</v>
       </c>
       <c r="F4" t="s">
-        <v>836</v>
+        <v>819</v>
       </c>
       <c r="G4" t="s">
-        <v>837</v>
+        <v>820</v>
       </c>
       <c r="H4" t="s">
-        <v>844</v>
+        <v>827</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -24415,33 +24695,101 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>784</v>
+        <v>768</v>
       </c>
       <c r="B7" t="s">
-        <v>930</v>
+        <v>953</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>820</v>
+        <v>803</v>
       </c>
       <c r="B10" t="s">
-        <v>821</v>
+        <v>804</v>
       </c>
       <c r="C10" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D10" t="s">
-        <v>819</v>
+        <v>802</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>915</v>
+      </c>
+      <c r="B11" t="s">
+        <v>916</v>
+      </c>
+      <c r="C11" t="s">
+        <v>609</v>
+      </c>
+      <c r="D11" t="s">
+        <v>802</v>
+      </c>
+      <c r="E11" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>918</v>
+      </c>
+      <c r="B12" t="s">
+        <v>919</v>
+      </c>
+      <c r="C12" t="s">
+        <v>609</v>
+      </c>
+      <c r="D12" t="s">
+        <v>802</v>
+      </c>
+      <c r="E12" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>920</v>
+      </c>
+      <c r="B13" t="s">
+        <v>921</v>
+      </c>
+      <c r="C13" t="s">
+        <v>609</v>
+      </c>
+      <c r="D13" t="s">
+        <v>802</v>
+      </c>
+      <c r="E13" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>922</v>
+      </c>
+      <c r="B14" t="s">
+        <v>923</v>
+      </c>
+      <c r="C14" t="s">
+        <v>609</v>
+      </c>
+      <c r="D14" t="s">
+        <v>802</v>
+      </c>
+      <c r="E14" t="s">
+        <v>917</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Excel for Module 7 TC012-017
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="982">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -2984,9 +2984,6 @@
     <t>TestMA Touch point Task-1</t>
   </si>
   <si>
-    <t>9/1/2021</t>
-  </si>
-  <si>
     <t>M7Task2</t>
   </si>
   <si>
@@ -2994,6 +2991,27 @@
   </si>
   <si>
     <t>9/4/2021</t>
+  </si>
+  <si>
+    <t>M7Task3</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Task-3</t>
+  </si>
+  <si>
+    <t>8/29/2021</t>
+  </si>
+  <si>
+    <t>9/6/2021</t>
+  </si>
+  <si>
+    <t>M7Task4</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Task-4</t>
+  </si>
+  <si>
+    <t>8/23/2021</t>
   </si>
 </sst>
 </file>
@@ -6524,10 +6542,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11065,7 +11083,7 @@
         <v>971</v>
       </c>
       <c r="E20" t="s">
-        <v>972</v>
+        <v>978</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>605</v>
@@ -11073,18 +11091,52 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>540</v>
       </c>
       <c r="C21" s="20" t="s">
+        <v>973</v>
+      </c>
+      <c r="E21" t="s">
         <v>974</v>
       </c>
-      <c r="E21" t="s">
+      <c r="I21" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>975</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="B22" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>976</v>
+      </c>
+      <c r="E22" t="s">
+        <v>977</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>979</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>980</v>
+      </c>
+      <c r="E23" t="s">
+        <v>981</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>605</v>
       </c>
     </row>
@@ -16801,8 +16853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:XFD42"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Excel for Module 7
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,47 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="24"/>
+    <workbookView activeTab="25" firstSheet="19" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
-    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
-    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
-    <sheet name="Entities" sheetId="3" r:id="rId4"/>
-    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
-    <sheet name="Test Custom Object" sheetId="23" r:id="rId6"/>
-    <sheet name="Fund" sheetId="7" r:id="rId7"/>
-    <sheet name="Deal" sheetId="4" r:id="rId8"/>
-    <sheet name="Fundraisings" sheetId="28" r:id="rId9"/>
-    <sheet name="DealRequestTracker" sheetId="14" r:id="rId10"/>
-    <sheet name="CustomSDG" sheetId="13" r:id="rId11"/>
-    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId12"/>
-    <sheet name="MarketingEvent" sheetId="15" r:id="rId13"/>
-    <sheet name="Partnerships" sheetId="8" r:id="rId14"/>
-    <sheet name="Commitments" sheetId="9" r:id="rId15"/>
-    <sheet name="Task" sheetId="12" r:id="rId16"/>
-    <sheet name="UploadImageData" sheetId="17" r:id="rId17"/>
-    <sheet name="Fields" sheetId="19" r:id="rId18"/>
-    <sheet name="Attendees" sheetId="20" r:id="rId19"/>
-    <sheet name="Deal Team" sheetId="21" r:id="rId20"/>
-    <sheet name="Coverages" sheetId="22" r:id="rId21"/>
-    <sheet name="SDGActions" sheetId="24" r:id="rId22"/>
-    <sheet name="Report" sheetId="25" r:id="rId23"/>
-    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId24"/>
-    <sheet name="Task1" sheetId="27" r:id="rId25"/>
-    <sheet name="Events" sheetId="29" r:id="rId26"/>
+    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
+    <sheet name="FieldSet" r:id="rId2" sheetId="1"/>
+    <sheet name="FieldComponent" r:id="rId3" sheetId="6"/>
+    <sheet name="Entities" r:id="rId4" sheetId="3"/>
+    <sheet name="Contacts" r:id="rId5" sheetId="2"/>
+    <sheet name="Test Custom Object" r:id="rId6" sheetId="23"/>
+    <sheet name="Fund" r:id="rId7" sheetId="7"/>
+    <sheet name="Deal" r:id="rId8" sheetId="4"/>
+    <sheet name="Fundraisings" r:id="rId9" sheetId="28"/>
+    <sheet name="DealRequestTracker" r:id="rId10" sheetId="14"/>
+    <sheet name="CustomSDG" r:id="rId11" sheetId="13"/>
+    <sheet name="ToggleButtonCheck" r:id="rId12" sheetId="16"/>
+    <sheet name="MarketingEvent" r:id="rId13" sheetId="15"/>
+    <sheet name="Partnerships" r:id="rId14" sheetId="8"/>
+    <sheet name="Commitments" r:id="rId15" sheetId="9"/>
+    <sheet name="Task" r:id="rId16" sheetId="12"/>
+    <sheet name="UploadImageData" r:id="rId17" sheetId="17"/>
+    <sheet name="Fields" r:id="rId18" sheetId="19"/>
+    <sheet name="Attendees" r:id="rId19" sheetId="20"/>
+    <sheet name="Deal Team" r:id="rId20" sheetId="21"/>
+    <sheet name="Coverages" r:id="rId21" sheetId="22"/>
+    <sheet name="SDGActions" r:id="rId22" sheetId="24"/>
+    <sheet name="Report" r:id="rId23" sheetId="25"/>
+    <sheet name="CustomEmailFolder" r:id="rId24" sheetId="26"/>
+    <sheet name="Task1" r:id="rId25" sheetId="27"/>
+    <sheet name="Events" r:id="rId26" sheetId="29"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1032">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3012,6 +3012,156 @@
   </si>
   <si>
     <t>8/23/2021</t>
+  </si>
+  <si>
+    <t>AAM7TestSamantha</t>
+  </si>
+  <si>
+    <t>AAM7TestJhon</t>
+  </si>
+  <si>
+    <t>AAM7TestKevin</t>
+  </si>
+  <si>
+    <t>Aleax</t>
+  </si>
+  <si>
+    <t>Dilger</t>
+  </si>
+  <si>
+    <t>M7CON4</t>
+  </si>
+  <si>
+    <t>M7CON5</t>
+  </si>
+  <si>
+    <t>M7CON6</t>
+  </si>
+  <si>
+    <t>M7Task5</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Call-1</t>
+  </si>
+  <si>
+    <t>navatariptesting+28101@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+70442@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+5497@gmail.com</t>
+  </si>
+  <si>
+    <t>M7Task6</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Call-2</t>
+  </si>
+  <si>
+    <t>9/7/2021</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Call-3</t>
+  </si>
+  <si>
+    <t>M7Task7</t>
+  </si>
+  <si>
+    <t>9/2/2021</t>
+  </si>
+  <si>
+    <t>M7Task8</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Call-4</t>
+  </si>
+  <si>
+    <t>TestTask LTP</t>
+  </si>
+  <si>
+    <t>M7Task9</t>
+  </si>
+  <si>
+    <t>M7Task10</t>
+  </si>
+  <si>
+    <t>TestCall LTP</t>
+  </si>
+  <si>
+    <t>M7CON7</t>
+  </si>
+  <si>
+    <t>AAM7TestOrko</t>
+  </si>
+  <si>
+    <t>navatariptesting+9709@gmail.com</t>
+  </si>
+  <si>
+    <t>M7CON9</t>
+  </si>
+  <si>
+    <t>M7CON10</t>
+  </si>
+  <si>
+    <t>M7CON8</t>
+  </si>
+  <si>
+    <t>AAM7TestEllie</t>
+  </si>
+  <si>
+    <t>AAM7TestJohr</t>
+  </si>
+  <si>
+    <t>AAM7TestKupes</t>
+  </si>
+  <si>
+    <t>Yatham</t>
+  </si>
+  <si>
+    <t>Dase</t>
+  </si>
+  <si>
+    <t>AAM7TestJenny</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>M7CON11</t>
+  </si>
+  <si>
+    <t>M7Event1</t>
+  </si>
+  <si>
+    <t>Start_Time</t>
+  </si>
+  <si>
+    <t>End_Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:30 PM </t>
+  </si>
+  <si>
+    <t>TestMA Touch point Event-1</t>
+  </si>
+  <si>
+    <t>navatariptesting+99747@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+74830@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+94558@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+62091@gmail.com</t>
+  </si>
+  <si>
+    <t>9/8/2021</t>
+  </si>
+  <si>
+    <t>9/9/2021</t>
   </si>
 </sst>
 </file>
@@ -3164,139 +3314,140 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="63">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="2" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3313,10 +3464,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3351,7 +3502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3386,7 +3537,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3480,21 +3631,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3511,7 +3662,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3563,15 +3714,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -3579,15 +3730,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="81.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3655,7 +3806,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row ht="75" r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>563</v>
       </c>
@@ -3797,17 +3948,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="L2"/>
+    <hyperlink r:id="rId2" ref="B5"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -3815,10 +3966,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
+    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3838,10 +3989,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -3887,14 +4038,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -3902,12 +4053,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="27.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="19.140625" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3927,7 +4078,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -3961,7 +4112,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>313</v>
       </c>
@@ -3995,7 +4146,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -4083,13 +4234,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -4097,13 +4248,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="12.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.5703125" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4126,7 +4277,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -4134,7 +4285,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
     </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -4207,16 +4358,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" r:id="rId1" ref="C5" tooltip="TestAzAlexa Deal"/>
+    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" r:id="rId2" ref="C4" tooltip="TestAzAlexa Info"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
@@ -4224,12 +4375,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="5" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
+    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4249,14 +4400,14 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
     </row>
-    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
@@ -4588,7 +4739,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="29" s="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -4617,14 +4768,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -4632,13 +4783,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -4652,10 +4803,10 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
     </row>
-    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>510</v>
@@ -4685,7 +4836,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>523</v>
@@ -4693,7 +4844,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
-    <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>767</v>
       </c>
@@ -4702,17 +4853,17 @@
       </c>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="10" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
     </row>
-    <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>524</v>
@@ -4720,7 +4871,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>444</v>
       </c>
@@ -4729,7 +4880,7 @@
       </c>
       <c r="C12" s="22"/>
     </row>
-    <row r="13" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>446</v>
       </c>
@@ -4739,13 +4890,13 @@
       <c r="C13" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -4753,26 +4904,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -4834,7 +4985,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
         <v>572</v>
@@ -4846,7 +4997,7 @@
       <c r="Q2" s="48"/>
       <c r="S2" s="48"/>
     </row>
-    <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
@@ -4907,7 +5058,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -4931,14 +5082,14 @@
       <c r="S7" s="16"/>
       <c r="T7" s="13"/>
     </row>
-    <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>448</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
-    <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>449</v>
       </c>
@@ -4946,13 +5097,13 @@
       <c r="C9" s="22"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -4960,12 +5111,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -4985,7 +5136,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
@@ -5077,7 +5228,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="15.75" r="15" s="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
@@ -5101,7 +5252,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="13"/>
     </row>
-    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="16" s="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>534</v>
       </c>
@@ -5118,7 +5269,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="17" s="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>539</v>
       </c>
@@ -5135,7 +5286,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>543</v>
       </c>
@@ -5156,13 +5307,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -5170,18 +5321,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="16.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="29" width="24.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="25.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -5298,13 +5449,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -5312,11 +5463,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5525,13 +5676,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -5539,8 +5690,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5745,13 +5896,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -5759,15 +5910,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -5787,7 +5938,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -5876,14 +6027,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -5891,8 +6042,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6146,13 +6297,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
@@ -6160,9 +6311,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6176,12 +6327,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>526</v>
@@ -6302,13 +6453,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -6316,10 +6467,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6342,7 +6493,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row ht="150" r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>553</v>
       </c>
@@ -6362,7 +6513,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+    <row ht="210" r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>558</v>
       </c>
@@ -6383,13 +6534,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -6397,13 +6548,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6450,14 +6601,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -6465,15 +6616,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6505,7 +6656,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>594</v>
       </c>
@@ -6534,34 +6685,34 @@
         <v>599</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMK29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD23"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="65.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="12" max="13" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -11140,28 +11291,120 @@
         <v>605</v>
       </c>
     </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>990</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>991</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>997</v>
+      </c>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>995</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>996</v>
+      </c>
+      <c r="E25" t="s">
+        <v>997</v>
+      </c>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>999</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>998</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E28" t="s">
+        <v>997</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E29" t="s">
+        <v>978</v>
+      </c>
+      <c r="I29" s="5"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMD11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AME13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="65.5703125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -11189,8 +11432,12 @@
       <c r="H1" s="21" t="s">
         <v>883</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="I1" s="31" t="s">
+        <v>1022</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>1023</v>
+      </c>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -12460,14 +12707,34 @@
         <v>895</v>
       </c>
     </row>
+    <row r="13" spans="1:1018" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1031</v>
+      </c>
+      <c r="I13" s="62">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1024</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
@@ -12475,15 +12742,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -13115,13 +13382,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALO74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALP74"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
       <selection activeCell="A73" sqref="A73:XFD74"/>
@@ -13129,11 +13396,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -14151,7 +14418,7 @@
       <c r="ALN1" s="5"/>
       <c r="ALO1" s="5"/>
     </row>
-    <row r="2" spans="1:1003" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -16357,7 +16624,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>523</v>
@@ -16387,7 +16654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="13.5" r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>611</v>
       </c>
@@ -16459,7 +16726,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="33" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>770</v>
       </c>
@@ -16484,22 +16751,22 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
     </row>
-    <row r="36" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="36" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
     </row>
-    <row r="37" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="37" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
     </row>
-    <row r="38" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="38" s="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>513</v>
@@ -16529,7 +16796,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="42" s="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>524</v>
@@ -16537,7 +16804,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="43" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>143</v>
       </c>
@@ -16548,7 +16815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="44" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>442</v>
       </c>
@@ -16557,13 +16824,13 @@
       </c>
       <c r="C44" s="22"/>
     </row>
-    <row r="46" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="46" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
       <c r="D46" s="53"/>
     </row>
-    <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="47" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>639</v>
@@ -16571,7 +16838,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="48" s="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>640</v>
       </c>
@@ -16825,7 +17092,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="73" s="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3" t="s">
         <v>955</v>
@@ -16845,30 +17112,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALS53"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E48" sqref="E45:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -17907,7 +18174,7 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
-    <row r="2" spans="1:1006" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="34" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -20112,7 +20379,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="18" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>506</v>
       </c>
@@ -20129,7 +20396,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="19" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>610</v>
       </c>
@@ -20143,7 +20410,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="20" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>766</v>
       </c>
@@ -20155,7 +20422,7 @@
       </c>
       <c r="E20" s="54"/>
     </row>
-    <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="21" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>769</v>
       </c>
@@ -20167,7 +20434,7 @@
       </c>
       <c r="E21" s="54"/>
     </row>
-    <row r="22" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="22" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E22" s="54"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -20395,7 +20662,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4" t="s">
@@ -20409,7 +20676,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="34" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>809</v>
       </c>
@@ -20426,7 +20693,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="35" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -20438,7 +20705,7 @@
       <c r="I35" s="53"/>
       <c r="J35" s="53"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4" t="s">
@@ -20452,7 +20719,7 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="38" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
         <v>958</v>
       </c>
@@ -20469,7 +20736,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="39" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
         <v>962</v>
       </c>
@@ -20486,7 +20753,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="13.5" r="40" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
         <v>966</v>
       </c>
@@ -20503,92 +20770,227 @@
         <v>969</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-    </row>
-    <row r="42" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4" t="s">
+    <row customFormat="1" r="41" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="50" t="s">
+        <v>987</v>
+      </c>
+      <c r="B41" s="50" t="s">
+        <v>983</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>985</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E41" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="42" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="50" t="s">
+        <v>988</v>
+      </c>
+      <c r="B42" s="50" t="s">
+        <v>982</v>
+      </c>
+      <c r="C42" s="50" t="s">
+        <v>273</v>
+      </c>
+      <c r="D42" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E42" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="43" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="50" t="s">
+        <v>989</v>
+      </c>
+      <c r="B43" s="50" t="s">
+        <v>984</v>
+      </c>
+      <c r="C43" s="50" t="s">
+        <v>986</v>
+      </c>
+      <c r="D43" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E43" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="44" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="50" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C44" s="50" t="s">
+        <v>736</v>
+      </c>
+      <c r="D44" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="45" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" s="50" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B45" s="50" t="s">
+        <v>1013</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>960</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="46" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" s="50" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B46" s="50" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="47" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" s="50" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B47" s="50" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C47" s="50" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="48" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" s="50" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B48" s="50" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C48" s="50" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="13.5" r="49" s="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D50" s="4"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>731</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B51" t="s">
         <v>732</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C51" t="s">
         <v>733</v>
       </c>
-      <c r="E44" s="60" t="s">
+      <c r="E51" s="60" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>735</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B52" t="s">
         <v>736</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C52" t="s">
         <v>737</v>
       </c>
-      <c r="E45" s="60" t="s">
+      <c r="E52" s="60" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>817</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B53" t="s">
         <v>818</v>
       </c>
-      <c r="E46" s="60"/>
-      <c r="K46" t="s">
+      <c r="E53" s="60"/>
+      <c r="K53" t="s">
         <v>555</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L53" t="s">
         <v>819</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M53" t="s">
         <v>820</v>
       </c>
-      <c r="N46" t="s">
+      <c r="N53" t="s">
         <v>821</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E44" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
-    <hyperlink ref="E45" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
-    <hyperlink ref="E38" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
-    <hyperlink ref="E39" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
-    <hyperlink ref="E40" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact01@gmail.com" r:id="rId1" ref="E51"/>
+    <hyperlink display="mailto:dealroom1.2+clientcontact13@gmail.com" r:id="rId2" ref="E52"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId3" ref="E38"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId4" ref="E39"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId5" ref="E40"/>
+    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId6" ref="E41"/>
+    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId7" ref="E42"/>
+    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId8" ref="E43"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -20596,9 +20998,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -20612,7 +21014,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -20641,13 +21043,13 @@
       <c r="C4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD9"/>
@@ -20655,19 +21057,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -20699,7 +21101,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -20711,7 +21113,7 @@
       <c r="I2" s="39"/>
       <c r="J2" s="41"/>
     </row>
-    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -20753,12 +21155,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="7" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="8" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -20772,7 +21174,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="9" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>507</v>
       </c>
@@ -20786,7 +21188,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="11" s="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -20800,7 +21202,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="12" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>144</v>
       </c>
@@ -20814,7 +21216,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="13" s="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>145</v>
       </c>
@@ -20857,13 +21259,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AML55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMM55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD20"/>
@@ -20871,15 +21273,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -21931,7 +22333,7 @@
       <c r="AMK1" s="6"/>
       <c r="AML1" s="6"/>
     </row>
-    <row r="2" spans="1:1026" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="2" s="44" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -22959,7 +23361,7 @@
       <c r="AMK2" s="43"/>
       <c r="AML2" s="43"/>
     </row>
-    <row r="3" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="3" s="1" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -24234,7 +24636,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="24" s="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -24245,7 +24647,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="25" s="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>146</v>
       </c>
@@ -24587,7 +24989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="52" s="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
@@ -24648,14 +25050,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD7"/>
@@ -24663,16 +25065,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -24734,7 +25136,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="6" s="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -24845,6 +25247,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel for Module 7 TC039-044
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1781" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="1039">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3162,6 +3162,27 @@
   </si>
   <si>
     <t>9/9/2021</t>
+  </si>
+  <si>
+    <t>M7Event2</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Event-2</t>
+  </si>
+  <si>
+    <t>9/5/2021</t>
+  </si>
+  <si>
+    <t>9/11/2021</t>
+  </si>
+  <si>
+    <t>M7Event3</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Event-3</t>
+  </si>
+  <si>
+    <t>9/12/2021</t>
   </si>
 </sst>
 </file>
@@ -11390,10 +11411,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AME13"/>
+  <dimension ref="A1:AME15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12726,6 +12747,42 @@
       <c r="J13" t="s">
         <v>1024</v>
       </c>
+    </row>
+    <row r="14" spans="1:1018" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1035</v>
+      </c>
+      <c r="I14" s="62">
+        <v>0.25</v>
+      </c>
+      <c r="J14" s="62">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1018" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D15" t="s">
+        <v>997</v>
+      </c>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Updated Excel for Module 7 TC045-055
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,47 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="25" firstSheet="19" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="FilePath" r:id="rId1" sheetId="18"/>
-    <sheet name="FieldSet" r:id="rId2" sheetId="1"/>
-    <sheet name="FieldComponent" r:id="rId3" sheetId="6"/>
-    <sheet name="Entities" r:id="rId4" sheetId="3"/>
-    <sheet name="Contacts" r:id="rId5" sheetId="2"/>
-    <sheet name="Test Custom Object" r:id="rId6" sheetId="23"/>
-    <sheet name="Fund" r:id="rId7" sheetId="7"/>
-    <sheet name="Deal" r:id="rId8" sheetId="4"/>
-    <sheet name="Fundraisings" r:id="rId9" sheetId="28"/>
-    <sheet name="DealRequestTracker" r:id="rId10" sheetId="14"/>
-    <sheet name="CustomSDG" r:id="rId11" sheetId="13"/>
-    <sheet name="ToggleButtonCheck" r:id="rId12" sheetId="16"/>
-    <sheet name="MarketingEvent" r:id="rId13" sheetId="15"/>
-    <sheet name="Partnerships" r:id="rId14" sheetId="8"/>
-    <sheet name="Commitments" r:id="rId15" sheetId="9"/>
-    <sheet name="Task" r:id="rId16" sheetId="12"/>
-    <sheet name="UploadImageData" r:id="rId17" sheetId="17"/>
-    <sheet name="Fields" r:id="rId18" sheetId="19"/>
-    <sheet name="Attendees" r:id="rId19" sheetId="20"/>
-    <sheet name="Deal Team" r:id="rId20" sheetId="21"/>
-    <sheet name="Coverages" r:id="rId21" sheetId="22"/>
-    <sheet name="SDGActions" r:id="rId22" sheetId="24"/>
-    <sheet name="Report" r:id="rId23" sheetId="25"/>
-    <sheet name="CustomEmailFolder" r:id="rId24" sheetId="26"/>
-    <sheet name="Task1" r:id="rId25" sheetId="27"/>
-    <sheet name="Events" r:id="rId26" sheetId="29"/>
+    <sheet name="FilePath" sheetId="18" r:id="rId1"/>
+    <sheet name="FieldSet" sheetId="1" r:id="rId2"/>
+    <sheet name="FieldComponent" sheetId="6" r:id="rId3"/>
+    <sheet name="Entities" sheetId="3" r:id="rId4"/>
+    <sheet name="Contacts" sheetId="2" r:id="rId5"/>
+    <sheet name="Test Custom Object" sheetId="23" r:id="rId6"/>
+    <sheet name="Fund" sheetId="7" r:id="rId7"/>
+    <sheet name="Deal" sheetId="4" r:id="rId8"/>
+    <sheet name="Fundraisings" sheetId="28" r:id="rId9"/>
+    <sheet name="DealRequestTracker" sheetId="14" r:id="rId10"/>
+    <sheet name="CustomSDG" sheetId="13" r:id="rId11"/>
+    <sheet name="ToggleButtonCheck" sheetId="16" r:id="rId12"/>
+    <sheet name="MarketingEvent" sheetId="15" r:id="rId13"/>
+    <sheet name="Partnerships" sheetId="8" r:id="rId14"/>
+    <sheet name="Commitments" sheetId="9" r:id="rId15"/>
+    <sheet name="Task" sheetId="12" r:id="rId16"/>
+    <sheet name="UploadImageData" sheetId="17" r:id="rId17"/>
+    <sheet name="Fields" sheetId="19" r:id="rId18"/>
+    <sheet name="Attendees" sheetId="20" r:id="rId19"/>
+    <sheet name="Deal Team" sheetId="21" r:id="rId20"/>
+    <sheet name="Coverages" sheetId="22" r:id="rId21"/>
+    <sheet name="SDGActions" sheetId="24" r:id="rId22"/>
+    <sheet name="Report" sheetId="25" r:id="rId23"/>
+    <sheet name="CustomEmailFolder" sheetId="26" r:id="rId24"/>
+    <sheet name="Task1" sheetId="27" r:id="rId25"/>
+    <sheet name="Events" sheetId="29" r:id="rId26"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1789" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="1068">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3161,9 +3161,6 @@
     <t>9/8/2021</t>
   </si>
   <si>
-    <t>9/9/2021</t>
-  </si>
-  <si>
     <t>M7Event2</t>
   </si>
   <si>
@@ -3182,7 +3179,97 @@
     <t>TestMA Touch point Event-3</t>
   </si>
   <si>
-    <t>9/12/2021</t>
+    <t>M7Task11</t>
+  </si>
+  <si>
+    <t>TestCall LTP1</t>
+  </si>
+  <si>
+    <t>9/13/2021</t>
+  </si>
+  <si>
+    <t>M7Task12</t>
+  </si>
+  <si>
+    <t>TestCall LTP2</t>
+  </si>
+  <si>
+    <t>M7Task13</t>
+  </si>
+  <si>
+    <t>MA Touch point Meeting-1</t>
+  </si>
+  <si>
+    <t>M7Task14</t>
+  </si>
+  <si>
+    <t>MA Touch point Meeting-2</t>
+  </si>
+  <si>
+    <t>M7Event4</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Event-4</t>
+  </si>
+  <si>
+    <t>9/20/2021</t>
+  </si>
+  <si>
+    <t>M7Event5</t>
+  </si>
+  <si>
+    <t>TestMA Touch point Event-5</t>
+  </si>
+  <si>
+    <t>M7Event6</t>
+  </si>
+  <si>
+    <t>TestEvent LTP1</t>
+  </si>
+  <si>
+    <t>M7Event7</t>
+  </si>
+  <si>
+    <t>TestEvent LTP2</t>
+  </si>
+  <si>
+    <t>9/14/2021</t>
+  </si>
+  <si>
+    <t>M7CON12</t>
+  </si>
+  <si>
+    <t>AAM7TestMindy</t>
+  </si>
+  <si>
+    <t>Kalling</t>
+  </si>
+  <si>
+    <t>M7CON13</t>
+  </si>
+  <si>
+    <t>AAM7TestParkar</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>M7CON14</t>
+  </si>
+  <si>
+    <t>AAM7TestShamim</t>
+  </si>
+  <si>
+    <t>wington</t>
+  </si>
+  <si>
+    <t>M7CON15</t>
+  </si>
+  <si>
+    <t>AAM7TestGreg</t>
+  </si>
+  <si>
+    <t>Beltzer</t>
   </si>
 </sst>
 </file>
@@ -3335,140 +3422,140 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="8" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="63">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="2" xfId="0">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="14" quotePrefix="1" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="3" fontId="2" numFmtId="49" xfId="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="2" xfId="0">
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="164" xfId="0">
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="1"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
-    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="2"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3485,10 +3572,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -3523,7 +3610,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3558,7 +3645,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3652,21 +3739,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -3683,7 +3770,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3735,15 +3822,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -3751,15 +3838,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="89.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="81.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="66.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3827,7 +3914,7 @@
         <v>566</v>
       </c>
     </row>
-    <row ht="75" r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>563</v>
       </c>
@@ -3969,17 +4056,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="L2"/>
-    <hyperlink r:id="rId2" ref="B5"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -3987,10 +4074,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="5" width="15.28515625" collapsed="true"/>
-    <col min="5" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4010,10 +4097,10 @@
         <v>93</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
-    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -4059,14 +4146,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
@@ -4074,12 +4161,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="27.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="20.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="19.140625" collapsed="true"/>
-    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4099,7 +4186,7 @@
         <v>310</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4133,7 +4220,7 @@
         <v>311</v>
       </c>
     </row>
-    <row ht="16.5" r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>313</v>
       </c>
@@ -4167,7 +4254,7 @@
         <v>775</v>
       </c>
     </row>
-    <row customFormat="1" r="9" s="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
@@ -4255,13 +4342,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
@@ -4269,13 +4356,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="22.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="18.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="5" width="12.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="32.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="127.5703125" collapsed="true"/>
-    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4298,7 +4385,7 @@
         <v>171</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="52"/>
@@ -4306,7 +4393,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="52"/>
     </row>
-    <row customFormat="1" r="3" s="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -4379,16 +4466,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" r:id="rId1" ref="C5" tooltip="TestAzAlexa Deal"/>
-    <hyperlink display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" r:id="rId2" ref="C4" tooltip="TestAzAlexa Info"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
@@ -4396,12 +4483,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="21.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="5" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="5" width="13.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="5" width="11.0" collapsed="true"/>
-    <col min="6" max="16384" style="5" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4421,14 +4508,14 @@
         <v>163</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="E2" s="51"/>
     </row>
-    <row customFormat="1" r="3" s="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="49" t="s">
@@ -4760,7 +4847,7 @@
         <v>345</v>
       </c>
     </row>
-    <row customFormat="1" r="29" s="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
@@ -4789,14 +4876,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
@@ -4804,13 +4891,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -4824,10 +4911,10 @@
         <v>64</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
     </row>
-    <row customFormat="1" r="3" s="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>510</v>
@@ -4857,7 +4944,7 @@
         <v>59</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9" t="s">
         <v>523</v>
@@ -4865,7 +4952,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
     </row>
-    <row customFormat="1" r="8" s="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>767</v>
       </c>
@@ -4874,17 +4961,17 @@
       </c>
       <c r="C8" s="22"/>
     </row>
-    <row customFormat="1" r="9" s="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
     </row>
-    <row customFormat="1" r="10" s="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
     </row>
-    <row customFormat="1" r="11" s="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
       <c r="B11" s="9" t="s">
         <v>524</v>
@@ -4892,7 +4979,7 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
     </row>
-    <row customFormat="1" r="12" s="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>444</v>
       </c>
@@ -4901,7 +4988,7 @@
       </c>
       <c r="C12" s="22"/>
     </row>
-    <row customFormat="1" r="13" s="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>446</v>
       </c>
@@ -4911,13 +4998,13 @@
       <c r="C13" s="22"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
@@ -4925,26 +5012,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -5006,7 +5093,7 @@
         <v>87</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="46" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" t="s">
         <v>572</v>
@@ -5018,7 +5105,7 @@
       <c r="Q2" s="48"/>
       <c r="S2" s="48"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="13"/>
@@ -5079,7 +5166,7 @@
         <v>91</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="13"/>
@@ -5103,14 +5190,14 @@
       <c r="S7" s="16"/>
       <c r="T7" s="13"/>
     </row>
-    <row customFormat="1" r="8" s="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>448</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
     </row>
-    <row customFormat="1" r="9" s="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>449</v>
       </c>
@@ -5118,13 +5205,13 @@
       <c r="C9" s="22"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
@@ -5132,12 +5219,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -5157,7 +5244,7 @@
         <v>548</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="13"/>
@@ -5249,7 +5336,7 @@
         <v>120</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="15" s="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="13"/>
@@ -5273,7 +5360,7 @@
       <c r="S15" s="16"/>
       <c r="T15" s="13"/>
     </row>
-    <row customFormat="1" r="16" s="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>534</v>
       </c>
@@ -5290,7 +5377,7 @@
         <v>538</v>
       </c>
     </row>
-    <row customFormat="1" r="17" s="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>539</v>
       </c>
@@ -5307,7 +5394,7 @@
         <v>542</v>
       </c>
     </row>
-    <row customFormat="1" r="18" s="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>543</v>
       </c>
@@ -5328,13 +5415,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -5342,18 +5429,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="29" width="16.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="29" width="24.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="25.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -5470,13 +5557,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
@@ -5484,11 +5571,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5697,13 +5784,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -5711,8 +5798,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5917,13 +6004,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -5931,15 +6018,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="77.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="32.85546875" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -5959,7 +6046,7 @@
         <v>45</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -6048,14 +6135,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -6063,8 +6150,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6318,13 +6405,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
@@ -6332,9 +6419,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6348,12 +6435,12 @@
         <v>14</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
       <c r="C2" s="53"/>
     </row>
-    <row customFormat="1" r="3" s="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="9" t="s">
         <v>526</v>
@@ -6474,13 +6561,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -6488,10 +6575,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6514,7 +6601,7 @@
         <v>552</v>
       </c>
     </row>
-    <row ht="150" r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>553</v>
       </c>
@@ -6534,7 +6621,7 @@
         <v>557</v>
       </c>
     </row>
-    <row ht="210" r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>558</v>
       </c>
@@ -6555,13 +6642,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -6569,13 +6656,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6622,14 +6709,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -6637,15 +6724,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6677,7 +6764,7 @@
         <v>593</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>594</v>
       </c>
@@ -6706,34 +6793,34 @@
         <v>599</v>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="65.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="12" max="13" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -11404,28 +11491,84 @@
       </c>
       <c r="I29" s="5"/>
     </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>1043</v>
+      </c>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AME15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMD19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="65.5703125" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -12739,7 +12882,7 @@
         <v>1030</v>
       </c>
       <c r="D13" t="s">
-        <v>1031</v>
+        <v>1039</v>
       </c>
       <c r="I13" s="62">
         <v>0</v>
@@ -12750,16 +12893,16 @@
     </row>
     <row r="14" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B14" t="s">
         <v>1032</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>1033</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>1034</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1035</v>
       </c>
       <c r="I14" s="62">
         <v>0.25</v>
@@ -12770,13 +12913,13 @@
     </row>
     <row r="15" spans="1:1018" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B15" t="s">
         <v>1036</v>
       </c>
-      <c r="B15" t="s">
-        <v>1037</v>
-      </c>
       <c r="C15" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D15" t="s">
         <v>997</v>
@@ -12784,14 +12927,75 @@
       <c r="I15" s="62"/>
       <c r="J15" s="62"/>
     </row>
+    <row r="16" spans="1:1018" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1039</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1048</v>
+      </c>
+      <c r="I16" s="62"/>
+      <c r="J16" s="62"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1039</v>
+      </c>
+      <c r="I17" s="62"/>
+      <c r="J17" s="62"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C18" t="s">
+        <v>974</v>
+      </c>
+      <c r="D18" t="s">
+        <v>997</v>
+      </c>
+      <c r="I18" s="62"/>
+      <c r="J18" s="62"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1034</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I19" s="62"/>
+      <c r="J19" s="62"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
@@ -12799,15 +13003,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -13439,13 +13643,13 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALP74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALO74"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
       <selection activeCell="A73" sqref="A73:XFD74"/>
@@ -13453,11 +13657,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -14475,7 +14679,7 @@
       <c r="ALN1" s="5"/>
       <c r="ALO1" s="5"/>
     </row>
-    <row customFormat="1" r="2" s="34" spans="1:1003" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1003" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="C2" s="33"/>
       <c r="D2" s="35"/>
@@ -16681,7 +16885,7 @@
         <v>285</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="3" t="s">
         <v>523</v>
@@ -16711,7 +16915,7 @@
         <v>32</v>
       </c>
     </row>
-    <row customHeight="1" ht="13.5" r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>611</v>
       </c>
@@ -16783,7 +16987,7 @@
         <v>931</v>
       </c>
     </row>
-    <row customFormat="1" r="33" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>770</v>
       </c>
@@ -16808,22 +17012,22 @@
         <v>76</v>
       </c>
     </row>
-    <row customFormat="1" r="35" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34"/>
       <c r="B35" s="20"/>
       <c r="C35" s="22"/>
     </row>
-    <row customFormat="1" r="36" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="22"/>
     </row>
-    <row customFormat="1" r="37" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="22"/>
     </row>
-    <row customFormat="1" r="38" s="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
         <v>513</v>
@@ -16853,7 +17057,7 @@
         <v>285</v>
       </c>
     </row>
-    <row customFormat="1" r="42" s="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>524</v>
@@ -16861,7 +17065,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row customFormat="1" r="43" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>143</v>
       </c>
@@ -16872,7 +17076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row customFormat="1" r="44" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>442</v>
       </c>
@@ -16881,13 +17085,13 @@
       </c>
       <c r="C44" s="22"/>
     </row>
-    <row customFormat="1" r="46" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
       <c r="D46" s="53"/>
     </row>
-    <row customFormat="1" r="47" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3" t="s">
         <v>639</v>
@@ -16895,7 +17099,7 @@
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row customFormat="1" r="48" s="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>640</v>
       </c>
@@ -17149,7 +17353,7 @@
         <v>32</v>
       </c>
     </row>
-    <row customFormat="1" r="73" s="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3" t="s">
         <v>955</v>
@@ -17169,30 +17373,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALS53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR58"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E48" sqref="E45:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -18231,7 +18435,7 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
-    <row customFormat="1" r="2" s="34" spans="1:1006" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1006" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -20436,7 +20640,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row customFormat="1" r="18" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>506</v>
       </c>
@@ -20453,7 +20657,7 @@
         <v>941</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="19" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>610</v>
       </c>
@@ -20467,7 +20671,7 @@
         <v>944</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="20" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>766</v>
       </c>
@@ -20479,7 +20683,7 @@
       </c>
       <c r="E20" s="54"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="21" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50" t="s">
         <v>769</v>
       </c>
@@ -20491,7 +20695,7 @@
       </c>
       <c r="E21" s="54"/>
     </row>
-    <row customFormat="1" r="22" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E22" s="54"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -20733,7 +20937,7 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row customFormat="1" r="34" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="50" t="s">
         <v>809</v>
       </c>
@@ -20750,7 +20954,7 @@
         <v>815</v>
       </c>
     </row>
-    <row customFormat="1" r="35" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="51"/>
       <c r="C35" s="51"/>
@@ -20762,292 +20966,372 @@
       <c r="I35" s="53"/>
       <c r="J35" s="53"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4" t="s">
         <v>955</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-    </row>
-    <row customFormat="1" r="38" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="4"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="50" t="s">
+        <v>958</v>
+      </c>
+      <c r="B37" s="50" t="s">
+        <v>959</v>
+      </c>
+      <c r="C37" s="50" t="s">
+        <v>960</v>
+      </c>
+      <c r="D37" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="50" t="s">
-        <v>958</v>
+        <v>962</v>
       </c>
       <c r="B38" s="50" t="s">
-        <v>959</v>
+        <v>963</v>
       </c>
       <c r="C38" s="50" t="s">
-        <v>960</v>
+        <v>964</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E38" s="22" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="39" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="50" t="s">
-        <v>962</v>
+        <v>966</v>
       </c>
       <c r="B39" s="50" t="s">
-        <v>963</v>
+        <v>967</v>
       </c>
       <c r="C39" s="50" t="s">
-        <v>964</v>
+        <v>968</v>
       </c>
       <c r="D39" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E39" s="22" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="40" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="50" t="s">
-        <v>966</v>
+        <v>987</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>967</v>
+        <v>983</v>
       </c>
       <c r="C40" s="50" t="s">
-        <v>968</v>
+        <v>985</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>957</v>
       </c>
-      <c r="E40" s="22" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row customFormat="1" r="41" s="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="50" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C41" s="50" t="s">
-        <v>985</v>
+        <v>273</v>
       </c>
       <c r="D41" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E41" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="42" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="50" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B42" s="50" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C42" s="50" t="s">
-        <v>273</v>
+        <v>986</v>
       </c>
       <c r="D42" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E42" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="43" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
-        <v>989</v>
+        <v>1007</v>
       </c>
       <c r="B43" s="50" t="s">
-        <v>984</v>
+        <v>1008</v>
       </c>
       <c r="C43" s="50" t="s">
-        <v>986</v>
+        <v>736</v>
       </c>
       <c r="D43" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E43" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="44" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="50" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c r="B44" s="50" t="s">
-        <v>1008</v>
+        <v>1013</v>
       </c>
       <c r="C44" s="50" t="s">
-        <v>736</v>
+        <v>960</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E44" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="45" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="50" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B45" s="50" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="C45" s="50" t="s">
-        <v>960</v>
+        <v>1016</v>
       </c>
       <c r="D45" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E45" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="46" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="50" t="s">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="C46" s="50" t="s">
-        <v>1016</v>
+        <v>1017</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E46" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="47" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="50" t="s">
-        <v>1011</v>
+        <v>1020</v>
       </c>
       <c r="B47" s="50" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
       <c r="C47" s="50" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="D47" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E47" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="48" s="50" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="50" t="s">
-        <v>1020</v>
+        <v>1056</v>
       </c>
       <c r="B48" s="50" t="s">
-        <v>1018</v>
+        <v>1057</v>
       </c>
       <c r="C48" s="50" t="s">
-        <v>1019</v>
+        <v>1058</v>
       </c>
       <c r="D48" s="22" t="s">
         <v>957</v>
       </c>
       <c r="E48" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="50" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B49" s="50" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C49" s="50" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="50" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B50" s="50" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C50" s="50" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D50" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="50" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B51" s="50" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D51" s="22" t="s">
+        <v>957</v>
+      </c>
+      <c r="E51" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="13.5" r="49" s="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4" t="s">
+    <row r="52" spans="1:14" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="53"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
+      <c r="D52" s="51"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="55"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+    </row>
+    <row r="54" spans="1:14" s="50" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4" t="s">
         <v>730</v>
       </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="D55" s="4"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>731</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B56" t="s">
         <v>732</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C56" t="s">
         <v>733</v>
       </c>
-      <c r="E51" s="60" t="s">
+      <c r="E56" s="60" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>735</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B57" t="s">
         <v>736</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C57" t="s">
         <v>737</v>
       </c>
-      <c r="E52" s="60" t="s">
+      <c r="E57" s="60" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>817</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B58" t="s">
         <v>818</v>
       </c>
-      <c r="E53" s="60"/>
-      <c r="K53" t="s">
+      <c r="E58" s="60"/>
+      <c r="K58" t="s">
         <v>555</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L58" t="s">
         <v>819</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M58" t="s">
         <v>820</v>
       </c>
-      <c r="N53" t="s">
+      <c r="N58" t="s">
         <v>821</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="mailto:dealroom1.2+clientcontact01@gmail.com" r:id="rId1" ref="E51"/>
-    <hyperlink display="mailto:dealroom1.2+clientcontact13@gmail.com" r:id="rId2" ref="E52"/>
-    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId3" ref="E38"/>
-    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId4" ref="E39"/>
-    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId5" ref="E40"/>
-    <hyperlink display="mailto:navatariptesting+11679@gmail.com" r:id="rId6" ref="E41"/>
-    <hyperlink display="mailto:navatariptesting+18785@gmail.com" r:id="rId7" ref="E42"/>
-    <hyperlink display="mailto:navatariptesting+49153@gmail.com" r:id="rId8" ref="E43"/>
+    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
@@ -21055,9 +21339,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -21071,7 +21355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="51"/>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -21100,13 +21384,13 @@
       <c r="C4" s="5"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD9"/>
@@ -21114,19 +21398,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -21158,7 +21442,7 @@
         <v>54</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39"/>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -21170,7 +21454,7 @@
       <c r="I2" s="39"/>
       <c r="J2" s="41"/>
     </row>
-    <row customFormat="1" r="3" s="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -21212,12 +21496,12 @@
         <v>90</v>
       </c>
     </row>
-    <row customFormat="1" r="7" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="D7" s="22"/>
       <c r="E7" s="22"/>
     </row>
-    <row customFormat="1" r="8" s="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -21231,7 +21515,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="11"/>
     </row>
-    <row customFormat="1" r="9" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>507</v>
       </c>
@@ -21245,7 +21529,7 @@
         <v>57</v>
       </c>
     </row>
-    <row customFormat="1" r="11" s="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -21259,7 +21543,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="11"/>
     </row>
-    <row customFormat="1" r="12" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>144</v>
       </c>
@@ -21273,7 +21557,7 @@
         <v>57</v>
       </c>
     </row>
-    <row customFormat="1" r="13" s="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>145</v>
       </c>
@@ -21316,13 +21600,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AML55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:XFD20"/>
@@ -21330,15 +21614,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
-    <col min="6" max="7" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -22390,7 +22674,7 @@
       <c r="AMK1" s="6"/>
       <c r="AML1" s="6"/>
     </row>
-    <row customFormat="1" r="2" s="44" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1026" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37"/>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
@@ -23418,7 +23702,7 @@
       <c r="AMK2" s="43"/>
       <c r="AML2" s="43"/>
     </row>
-    <row customFormat="1" r="3" s="1" spans="1:1026" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -24693,7 +24977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row customFormat="1" r="24" s="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -24704,7 +24988,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="3"/>
     </row>
-    <row customFormat="1" r="25" s="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>146</v>
       </c>
@@ -25046,7 +25330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row customFormat="1" r="52" s="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
@@ -25107,14 +25391,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD7"/>
@@ -25122,16 +25406,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>9</v>
       </c>
@@ -25193,7 +25477,7 @@
         <v>827</v>
       </c>
     </row>
-    <row customFormat="1" r="6" s="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
@@ -25304,6 +25588,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel for Module 7 TC055-070
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1881" uniqueCount="1094">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3270,6 +3270,84 @@
   </si>
   <si>
     <t>Beltzer</t>
+  </si>
+  <si>
+    <t>M8Field1</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deal Sample 1 </t>
+  </si>
+  <si>
+    <t>M8Field2</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Deal sample 2</t>
+  </si>
+  <si>
+    <t>M8Field3</t>
+  </si>
+  <si>
+    <t>Deal Sample Test New 12345:"&gt;&lt;?/!@#$</t>
+  </si>
+  <si>
+    <t>M8Field4</t>
+  </si>
+  <si>
+    <t>Text Area</t>
+  </si>
+  <si>
+    <t>Deal Sample Test New12345628-04-2021:"?&gt;&lt;/!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>M8Field5</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Deal sample Dependent test new field123456:"??&gt;&lt;&lt;!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>M8Field6</t>
+  </si>
+  <si>
+    <t>Lookup Relationship</t>
+  </si>
+  <si>
+    <t>Deal sample Dependent test new field123456:"?&gt;&lt;!@#$%^&amp;*()1234567890123456789!@#$%^&amp;*()</t>
+  </si>
+  <si>
+    <t>9/17/2021</t>
+  </si>
+  <si>
+    <t>M7Task15</t>
+  </si>
+  <si>
+    <t>MA Touch point Meeting-3</t>
+  </si>
+  <si>
+    <t>M7Task16</t>
+  </si>
+  <si>
+    <t>MA Touch point Meeting-4</t>
+  </si>
+  <si>
+    <t>M7Task17</t>
+  </si>
+  <si>
+    <t>TestTask LTPP</t>
+  </si>
+  <si>
+    <t>M7Task18</t>
+  </si>
+  <si>
+    <t>TestMeeting LTP</t>
   </si>
 </sst>
 </file>
@@ -6801,10 +6879,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ33"/>
+  <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11531,7 +11609,12 @@
       <c r="C32" s="20" t="s">
         <v>1043</v>
       </c>
-      <c r="I32" s="5"/>
+      <c r="E32" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
@@ -11543,9 +11626,68 @@
       <c r="C33" s="20" t="s">
         <v>1045</v>
       </c>
+      <c r="E33" t="s">
+        <v>1085</v>
+      </c>
       <c r="I33" s="5" t="s">
         <v>605</v>
       </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1034</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>1088</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>1091</v>
+      </c>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>1092</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E37" t="s">
+        <v>978</v>
+      </c>
+      <c r="I37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12995,10 +13137,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13639,6 +13781,102 @@
       </c>
       <c r="G38" t="s">
         <v>405</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1083</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1084</v>
       </c>
     </row>
   </sheetData>
@@ -17381,7 +17619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALR58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update field component of module 8
Signed-off-by: Ravi
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22689FD1-E4FE-46E7-AC2F-247C6A037CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="24"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -3320,9 +3321,6 @@
     <t>Lookup Relationship</t>
   </si>
   <si>
-    <t>Deal sample Dependent test new field123456:"?&gt;&lt;!@#$%^&amp;*()1234567890123456789!@#$%^&amp;*()</t>
-  </si>
-  <si>
     <t>9/17/2021</t>
   </si>
   <si>
@@ -3348,12 +3346,15 @@
   </si>
   <si>
     <t>TestMeeting LTP</t>
+  </si>
+  <si>
+    <t>Deal sample :"?&gt;&lt;!@#$%^&amp;*()1234567890123456789!@#$%^&amp;*()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -3630,7 +3631,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3907,7 +3908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3916,15 +3917,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4134,8 +4135,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4143,19 +4144,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.125" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4230,21 +4231,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4425,22 +4426,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.125" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.125" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4544,29 +4545,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.625" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4960,7 +4961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4969,8 +4970,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -5081,7 +5082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5090,23 +5091,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5288,7 +5289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5297,9 +5298,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -5498,7 +5499,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5507,15 +5508,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.25" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5640,7 +5641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -5649,11 +5650,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5867,7 +5868,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5876,8 +5877,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6087,7 +6088,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -6096,12 +6097,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6219,7 +6220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6228,8 +6229,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6488,7 +6489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6497,9 +6498,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6644,7 +6645,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6653,9 +6654,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -6725,7 +6726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6734,13 +6735,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6793,7 +6794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6802,15 +6803,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" collapsed="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.125" collapsed="1"/>
+    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6878,27 +6879,27 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:AMJ37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.75" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -11627,7 +11628,7 @@
         <v>1045</v>
       </c>
       <c r="E33" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="I33" s="5" t="s">
         <v>605</v>
@@ -11635,13 +11636,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B34" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="E34" t="s">
         <v>1034</v>
@@ -11652,13 +11653,13 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B35" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>605</v>
@@ -11666,13 +11667,13 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B36" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>605</v>
@@ -11680,13 +11681,13 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>535</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E37" t="s">
         <v>978</v>
@@ -11701,7 +11702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:AMD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11710,13 +11711,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -13142,21 +13143,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.25" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -13882,7 +13883,7 @@
         <v>1083</v>
       </c>
       <c r="D47" t="s">
-        <v>1084</v>
+        <v>1093</v>
       </c>
     </row>
   </sheetData>
@@ -13892,7 +13893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:ALO74"/>
   <sheetViews>
     <sheetView topLeftCell="A59" workbookViewId="0">
@@ -13901,11 +13902,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -17622,7 +17623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:ALR58"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
@@ -17631,16 +17632,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.75" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -21560,21 +21561,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
-    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
-    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
-    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
-    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
-    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
-    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
-    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21583,9 +21584,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -21633,7 +21634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21642,16 +21643,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -21849,7 +21850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AML55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21858,12 +21859,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -25641,7 +25642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25650,13 +25651,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Excel for Smoke TC related to CT
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Namita\git\einstein-code-version-2-pe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Navatar\git\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22689FD1-E4FE-46E7-AC2F-247C6A037CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="19" activeTab="25"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1884" uniqueCount="1094">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1110">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3350,11 +3349,59 @@
   <si>
     <t>Deal sample :"?&gt;&lt;!@#$%^&amp;*()1234567890123456789!@#$%^&amp;*()</t>
   </si>
+  <si>
+    <t>Smoke</t>
+  </si>
+  <si>
+    <t>SMOKECTINS</t>
+  </si>
+  <si>
+    <t>SmokeTest Instituion-1</t>
+  </si>
+  <si>
+    <t>SMOKECTINS2</t>
+  </si>
+  <si>
+    <t>SmokeCTTest Instituion-1</t>
+  </si>
+  <si>
+    <t>SMOKECTINS3</t>
+  </si>
+  <si>
+    <t>SmokeCTTest Instituion-2</t>
+  </si>
+  <si>
+    <t>SMOKECTCON1</t>
+  </si>
+  <si>
+    <t>SmokeTest</t>
+  </si>
+  <si>
+    <t>Contact-1</t>
+  </si>
+  <si>
+    <t>SmokeCTTask1</t>
+  </si>
+  <si>
+    <t>SmokeTest Task-1</t>
+  </si>
+  <si>
+    <t>SmokeCTLogACall1</t>
+  </si>
+  <si>
+    <t>SmokeTest Log a call -1</t>
+  </si>
+  <si>
+    <t>SmokeCTEvent1</t>
+  </si>
+  <si>
+    <t>SmokeTest Event-1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
@@ -3631,7 +3678,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3908,7 +3955,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3917,15 +3964,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="81.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="34.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="89.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="66" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4135,8 +4182,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -4144,19 +4191,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="15.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="15.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4231,21 +4278,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="27.25" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4426,22 +4473,22 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="127.625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.140625" style="5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="127.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -4545,29 +4592,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view" xr:uid="{00000000-0004-0000-0B00-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId1" tooltip="TestAzAlexa Deal" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/a0F8A000002tJdiUAE/view"/>
+    <hyperlink ref="C4" r:id="rId2" tooltip="TestAzAlexa Info" display="https://navatar-5b--sb13.lightning.force.com/lightning/r/0018A00000gk11EQAQ/view"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.625" style="5" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.75" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="11" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="9.125" style="5" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="5" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4961,7 +5008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4970,8 +5017,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -5082,7 +5129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5091,23 +5138,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="27.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="14" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5289,7 +5336,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5298,9 +5345,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="32" customFormat="1" x14ac:dyDescent="0.25">
@@ -5499,7 +5546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5508,15 +5555,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.125" style="29" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.25" style="29" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="25.375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.140625" style="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.28515625" style="29" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -5641,7 +5688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -5650,11 +5697,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5868,7 +5915,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5877,8 +5924,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6088,7 +6135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -6097,12 +6144,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="77.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6220,7 +6267,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6229,8 +6276,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6489,7 +6536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6498,9 +6545,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6645,7 +6692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6654,9 +6701,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -6726,7 +6773,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6735,13 +6782,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="21.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6794,7 +6841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6803,15 +6850,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" collapsed="1"/>
-    <col min="2" max="2" width="28.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="29.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.140625" collapsed="1"/>
+    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6879,27 +6926,27 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:AMJ37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="26.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
@@ -11696,28 +11743,55 @@
         <v>605</v>
       </c>
     </row>
+    <row r="40" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="20" t="s">
+        <v>1105</v>
+      </c>
+      <c r="H41" t="s">
+        <v>541</v>
+      </c>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B42" s="19"/>
+      <c r="C42" s="20" t="s">
+        <v>1107</v>
+      </c>
+      <c r="H42" t="s">
+        <v>541</v>
+      </c>
+      <c r="I42" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
-  <dimension ref="A1:AMD19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AMD22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="65.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="65.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="24.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="8.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1018" x14ac:dyDescent="0.25">
@@ -13137,27 +13211,49 @@
       <c r="I19" s="62"/>
       <c r="J19" s="62"/>
     </row>
+    <row r="21" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="32" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1109</v>
+      </c>
+      <c r="H22" t="s">
+        <v>886</v>
+      </c>
+      <c r="I22" s="62">
+        <v>0</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1024</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.25" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -13893,20 +13989,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:ALO74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALO79"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:XFD74"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76:XFD79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
@@ -17617,31 +17713,72 @@
         <v>32</v>
       </c>
     </row>
+    <row r="76" spans="1:4" s="32" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C77" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C79" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:ALR58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ALR61"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="17.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.75" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.75" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -21559,23 +21696,54 @@
         <v>821</v>
       </c>
     </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4" t="s">
+        <v>1094</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1103</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1029</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="E56" r:id="rId1" display="mailto:dealroom1.2+clientcontact01@gmail.com"/>
+    <hyperlink ref="E57" r:id="rId2" display="mailto:dealroom1.2+clientcontact13@gmail.com"/>
+    <hyperlink ref="E37" r:id="rId3" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E38" r:id="rId4" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E39" r:id="rId5" display="mailto:navatariptesting+49153@gmail.com"/>
+    <hyperlink ref="E40" r:id="rId6" display="mailto:navatariptesting+11679@gmail.com"/>
+    <hyperlink ref="E41" r:id="rId7" display="mailto:navatariptesting+18785@gmail.com"/>
+    <hyperlink ref="E42" r:id="rId8" display="mailto:navatariptesting+49153@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21584,9 +21752,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -21634,7 +21802,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21643,16 +21811,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="21" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -21850,7 +22018,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21859,12 +22027,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="24.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="12.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -25642,7 +25810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25651,13 +25819,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated Excel for TC079-093 of Smoke
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2125" uniqueCount="1245">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3776,9 +3776,6 @@
     <t>SMOKEDEALCON1</t>
   </si>
   <si>
-    <t>navatariptesting+1388@gmail.com</t>
-  </si>
-  <si>
     <t>SmokeTestNavatar</t>
   </si>
   <si>
@@ -3786,6 +3783,24 @@
   </si>
   <si>
     <t>SMOKEDEAL2</t>
+  </si>
+  <si>
+    <t>SMOKEPFCON1</t>
+  </si>
+  <si>
+    <t>SMOKEFR1</t>
+  </si>
+  <si>
+    <t>SmokeTest Fundraising1</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>SMOKEFUND3</t>
+  </si>
+  <si>
+    <t>SmokeTest Fund1</t>
   </si>
 </sst>
 </file>
@@ -14466,7 +14481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALP103"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
@@ -18546,7 +18561,7 @@
   <dimension ref="A1:ALR71"/>
   <sheetViews>
     <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+      <selection activeCell="A69" sqref="A69:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22691,10 +22706,10 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B71" t="s">
         <v>1236</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1237</v>
       </c>
       <c r="C71" t="s">
         <v>106</v>
@@ -22780,10 +22795,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23013,6 +23028,20 @@
         <v>1202</v>
       </c>
     </row>
+    <row r="24" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23022,8 +23051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D81" sqref="D80:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26997,7 +27026,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>1228</v>
@@ -27009,7 +27038,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>1232</v>
@@ -27028,10 +27057,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27243,6 +27272,28 @@
         <v>1199</v>
       </c>
     </row>
+    <row r="18" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1241</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1242</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Excel for TC096-098
Signed-off-by: Azhar
</commit_message>
<xml_diff>
--- a/Phase1DataSheet - Copy.xlsx
+++ b/Phase1DataSheet - Copy.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="926" firstSheet="14" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="FilePath" sheetId="18" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="CustomEmailFolder" sheetId="26" r:id="rId24"/>
     <sheet name="Task1" sheetId="27" r:id="rId25"/>
     <sheet name="Events" sheetId="29" r:id="rId26"/>
+    <sheet name="MI" sheetId="30" r:id="rId27"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="1240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2133" uniqueCount="1249">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -3776,9 +3777,6 @@
     <t>SMOKEDEALCON1</t>
   </si>
   <si>
-    <t>navatariptesting+1388@gmail.com</t>
-  </si>
-  <si>
     <t>SmokeTestNavatar</t>
   </si>
   <si>
@@ -3786,6 +3784,36 @@
   </si>
   <si>
     <t>SMOKEDEAL2</t>
+  </si>
+  <si>
+    <t>SMOKEPFCON1</t>
+  </si>
+  <si>
+    <t>SMOKEFR1</t>
+  </si>
+  <si>
+    <t>SmokeTest Fundraising1</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>SMOKEFUND3</t>
+  </si>
+  <si>
+    <t>SmokeTest Fund1</t>
+  </si>
+  <si>
+    <t>SMOKCON9</t>
+  </si>
+  <si>
+    <t>Marketing_InitiativeName</t>
+  </si>
+  <si>
+    <t>SmokeMI1</t>
+  </si>
+  <si>
+    <t>M1TestMarketingInitiative</t>
   </si>
 </sst>
 </file>
@@ -13712,6 +13740,41 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
@@ -14466,7 +14529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ALP103"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
@@ -18543,10 +18606,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ALR71"/>
+  <dimension ref="A1:ALR72"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61:XFD61"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22659,47 +22722,61 @@
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
-        <v>1099</v>
+      <c r="A69" t="s">
+        <v>1245</v>
       </c>
       <c r="B69" t="s">
-        <v>1100</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
         <v>1101</v>
       </c>
-      <c r="D69" s="22" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E69" t="s">
-        <v>1027</v>
+      <c r="D69" t="s">
+        <v>1211</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1235</v>
+      <c r="A70" s="32" t="s">
+        <v>1099</v>
       </c>
       <c r="B70" t="s">
         <v>1100</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>1101</v>
       </c>
       <c r="D70" s="22" t="s">
-        <v>1230</v>
+        <v>1094</v>
+      </c>
+      <c r="E70" t="s">
+        <v>1027</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="B71" t="s">
-        <v>1237</v>
+        <v>1100</v>
       </c>
       <c r="C71" t="s">
         <v>106</v>
       </c>
       <c r="D71" s="22" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="22" t="s">
         <v>1234</v>
       </c>
     </row>
@@ -22780,10 +22857,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23013,6 +23090,20 @@
         <v>1202</v>
       </c>
     </row>
+    <row r="24" spans="1:10" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D24" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23022,8 +23113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMM71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="D81" sqref="D80:D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26997,7 +27088,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C70" s="22" t="s">
         <v>1228</v>
@@ -27009,7 +27100,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C71" s="22" t="s">
         <v>1232</v>
@@ -27028,10 +27119,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="A18" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27243,6 +27334,28 @@
         <v>1199</v>
       </c>
     </row>
+    <row r="18" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>1092</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1241</v>
+      </c>
+      <c r="J19" t="s">
+        <v>1242</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>